<commit_message>
Changes to be committed: 	modified:   algotrader-repo/main.py 	modified:   algotrader-repo/models/downprojection/expected_returns_90d.xlsx 	modified:   algotrader-repo/src/utils/ulits.py 	modified:   algotrader-repo/src/visualization/visualize.py
</commit_message>
<xml_diff>
--- a/algotrader-repo/models/downprojection/expected_returns_90d.xlsx
+++ b/algotrader-repo/models/downprojection/expected_returns_90d.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I35"/>
+  <dimension ref="A1:P35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -474,6 +474,41 @@
           <t>p_value</t>
         </is>
       </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>ref_min_val</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>ref_q1</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>ref_median_val</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>ref_mean_val</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>ref_q3</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>ref_max_val</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>ref_n</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -482,28 +517,49 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.1265049616545293</v>
+        <v>-0.1265050405302508</v>
       </c>
       <c r="C2" t="n">
-        <v>0.02798747888241314</v>
+        <v>0.02798740803096483</v>
       </c>
       <c r="D2" t="n">
-        <v>0.1102870488546577</v>
+        <v>0.1175778209339658</v>
       </c>
       <c r="E2" t="n">
-        <v>0.09469484665804329</v>
+        <v>0.09510147717839937</v>
       </c>
       <c r="F2" t="n">
-        <v>0.1634688346927461</v>
+        <v>0.1633665301904315</v>
       </c>
       <c r="G2" t="n">
-        <v>0.3411567172740176</v>
+        <v>0.3411567014648403</v>
       </c>
       <c r="H2" t="n">
         <v>200</v>
       </c>
       <c r="I2" t="n">
-        <v>3.764955486754722e-22</v>
+        <v>0.0004234621523382656</v>
+      </c>
+      <c r="J2" t="n">
+        <v>-0.7128912276988006</v>
+      </c>
+      <c r="K2" t="n">
+        <v>-0.008995531115022078</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0.09670145975948755</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0.0877476370511667</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0.1946853083055953</v>
+      </c>
+      <c r="O2" t="n">
+        <v>0.799091992791544</v>
+      </c>
+      <c r="P2" t="n">
+        <v>6906</v>
       </c>
     </row>
     <row r="3">
@@ -513,16 +569,16 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-0.9963285875401667</v>
+        <v>-1.004254528637929</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.4736300863659823</v>
+        <v>-0.5450151586209133</v>
       </c>
       <c r="D3" t="n">
-        <v>0.233089317198891</v>
+        <v>-0.04893837032341358</v>
       </c>
       <c r="E3" t="n">
-        <v>0.8270918184559203</v>
+        <v>0.8120696717870111</v>
       </c>
       <c r="F3" t="n">
         <v>2.362868664365059</v>
@@ -534,7 +590,28 @@
         <v>200</v>
       </c>
       <c r="I3" t="n">
-        <v>1.408206522500153e-37</v>
+        <v>1.502334513986329e-19</v>
+      </c>
+      <c r="J3" t="n">
+        <v>-1.970100851827858</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.5094108636703494</v>
+      </c>
+      <c r="L3" t="n">
+        <v>2.362868664365059</v>
+      </c>
+      <c r="M3" t="n">
+        <v>1.632517749329234</v>
+      </c>
+      <c r="N3" t="n">
+        <v>2.362868664365059</v>
+      </c>
+      <c r="O3" t="n">
+        <v>2.828942759145652</v>
+      </c>
+      <c r="P3" t="n">
+        <v>6910</v>
       </c>
     </row>
     <row r="4">
@@ -547,25 +624,46 @@
         <v>-0.1606715517021195</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0004906264221942103</v>
+        <v>0.0004905227649435368</v>
       </c>
       <c r="D4" t="n">
-        <v>0.04884288860317222</v>
+        <v>0.04884297901244362</v>
       </c>
       <c r="E4" t="n">
-        <v>0.04932461614565239</v>
+        <v>0.0469784436399546</v>
       </c>
       <c r="F4" t="n">
-        <v>0.1283519713295232</v>
+        <v>0.1305233328569811</v>
       </c>
       <c r="G4" t="n">
-        <v>0.2284211661951383</v>
+        <v>0.2475528231697341</v>
       </c>
       <c r="H4" t="n">
         <v>200</v>
       </c>
       <c r="I4" t="n">
-        <v>1.538731734313633e-52</v>
+        <v>1.765419703784751e-21</v>
+      </c>
+      <c r="J4" t="n">
+        <v>-0.6917923287221859</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.0004905227649435368</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0.0004905227649435368</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0.0112558562944327</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0.03333001620224238</v>
+      </c>
+      <c r="O4" t="n">
+        <v>0.6536035888920079</v>
+      </c>
+      <c r="P4" t="n">
+        <v>6906</v>
       </c>
     </row>
     <row r="5">
@@ -581,22 +679,43 @@
         <v>-0.04226984730491904</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.02864099755155148</v>
+        <v>-0.02817055315158657</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.01971962389684245</v>
+        <v>-0.01953953227856854</v>
       </c>
       <c r="F5" t="n">
-        <v>0.007571078693451479</v>
+        <v>0.006865740074103668</v>
       </c>
       <c r="G5" t="n">
-        <v>0.0652777555487314</v>
+        <v>0.06904032557960171</v>
       </c>
       <c r="H5" t="n">
         <v>200</v>
       </c>
       <c r="I5" t="n">
-        <v>8.159023794354062e-67</v>
+        <v>3.890157063537524e-24</v>
+      </c>
+      <c r="J5" t="n">
+        <v>-0.480714522359086</v>
+      </c>
+      <c r="K5" t="n">
+        <v>-0.02870262439855314</v>
+      </c>
+      <c r="L5" t="n">
+        <v>-0.004286593184065727</v>
+      </c>
+      <c r="M5" t="n">
+        <v>-0.001769025086395777</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0.02702615387901008</v>
+      </c>
+      <c r="O5" t="n">
+        <v>1.804759915703559</v>
+      </c>
+      <c r="P5" t="n">
+        <v>6909</v>
       </c>
     </row>
     <row r="6">
@@ -609,25 +728,46 @@
         <v>-0.5741156638068546</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.246349304766334</v>
+        <v>-0.2608960287093573</v>
       </c>
       <c r="D6" t="n">
-        <v>1.059753979359459</v>
+        <v>0.7461733332485138</v>
       </c>
       <c r="E6" t="n">
-        <v>0.5917803243866386</v>
+        <v>0.5866907526832866</v>
       </c>
       <c r="F6" t="n">
         <v>1.402726308520786</v>
       </c>
       <c r="G6" t="n">
-        <v>1.885756039738988</v>
+        <v>1.97926389297824</v>
       </c>
       <c r="H6" t="n">
         <v>200</v>
       </c>
       <c r="I6" t="n">
-        <v>2.057077244726661e-34</v>
+        <v>1.381025224912823e-22</v>
+      </c>
+      <c r="J6" t="n">
+        <v>-0.8465190237872344</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0.4181442436478377</v>
+      </c>
+      <c r="L6" t="n">
+        <v>1.402726308520786</v>
+      </c>
+      <c r="M6" t="n">
+        <v>1.01457803255993</v>
+      </c>
+      <c r="N6" t="n">
+        <v>1.402726308520786</v>
+      </c>
+      <c r="O6" t="n">
+        <v>2.754279508674765</v>
+      </c>
+      <c r="P6" t="n">
+        <v>6910</v>
       </c>
     </row>
     <row r="7">
@@ -637,28 +777,49 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-0.6946201834772257</v>
+        <v>-0.8494158351574298</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.1371200267668487</v>
+        <v>-0.1399514935542799</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.001980198748664537</v>
+        <v>-0.01164840865164129</v>
       </c>
       <c r="E7" t="n">
-        <v>0.05054577296465212</v>
+        <v>0.04706193396998795</v>
       </c>
       <c r="F7" t="n">
-        <v>0.2446032136035799</v>
+        <v>0.2732943658675587</v>
       </c>
       <c r="G7" t="n">
-        <v>0.9796679077486566</v>
+        <v>1.133634764220366</v>
       </c>
       <c r="H7" t="n">
         <v>200</v>
       </c>
       <c r="I7" t="n">
-        <v>5.720708493511347e-86</v>
+        <v>4.11580350674338e-31</v>
+      </c>
+      <c r="J7" t="n">
+        <v>-0.971184982592862</v>
+      </c>
+      <c r="K7" t="n">
+        <v>-0.3352642187046779</v>
+      </c>
+      <c r="L7" t="n">
+        <v>-0.3352642187046779</v>
+      </c>
+      <c r="M7" t="n">
+        <v>-0.1152649432677471</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0.07039262924546211</v>
+      </c>
+      <c r="O7" t="n">
+        <v>1.694114229814654</v>
+      </c>
+      <c r="P7" t="n">
+        <v>6910</v>
       </c>
     </row>
     <row r="8">
@@ -668,28 +829,49 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-0.05384876024834782</v>
+        <v>-0.05247635345385821</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.02002263021299156</v>
+        <v>-0.01956554635081176</v>
       </c>
       <c r="D8" t="n">
         <v>-0.001315350380615605</v>
       </c>
       <c r="E8" t="n">
-        <v>0.002951663859760121</v>
+        <v>0.003357729475243577</v>
       </c>
       <c r="F8" t="n">
-        <v>0.01324836998480487</v>
+        <v>0.01283630487301207</v>
       </c>
       <c r="G8" t="n">
-        <v>0.09716186446069816</v>
+        <v>0.1054033449155986</v>
       </c>
       <c r="H8" t="n">
         <v>200</v>
       </c>
       <c r="I8" t="n">
-        <v>2.498722738061117e-60</v>
+        <v>0.003478627471606414</v>
+      </c>
+      <c r="J8" t="n">
+        <v>-0.2585007380338438</v>
+      </c>
+      <c r="K8" t="n">
+        <v>-0.02388755105583503</v>
+      </c>
+      <c r="L8" t="n">
+        <v>-0.0002142456511333328</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0.001136466846099111</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0.02693515558715022</v>
+      </c>
+      <c r="O8" t="n">
+        <v>0.1450303875968654</v>
+      </c>
+      <c r="P8" t="n">
+        <v>6910</v>
       </c>
     </row>
     <row r="9">
@@ -699,19 +881,19 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-0.4675572303591928</v>
+        <v>-0.5288696539920751</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.04304517383531806</v>
+        <v>-0.0307400945708086</v>
       </c>
       <c r="D9" t="n">
-        <v>0.04193360490271703</v>
+        <v>0.05215938453877618</v>
       </c>
       <c r="E9" t="n">
-        <v>0.03352604280175224</v>
+        <v>0.03375089676710478</v>
       </c>
       <c r="F9" t="n">
-        <v>0.09778557847554323</v>
+        <v>0.101760537121894</v>
       </c>
       <c r="G9" t="n">
         <v>0.2933914744316351</v>
@@ -720,7 +902,28 @@
         <v>200</v>
       </c>
       <c r="I9" t="n">
-        <v>3.144564538434882e-42</v>
+        <v>0.00735236862467733</v>
+      </c>
+      <c r="J9" t="n">
+        <v>-1.734894842769978</v>
+      </c>
+      <c r="K9" t="n">
+        <v>-0.07961270423142532</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0.03981301103870794</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0.01098484635283651</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0.1400376213150778</v>
+      </c>
+      <c r="O9" t="n">
+        <v>1.405342566876112</v>
+      </c>
+      <c r="P9" t="n">
+        <v>6906</v>
       </c>
     </row>
     <row r="10">
@@ -730,28 +933,49 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-0.07762348100014951</v>
+        <v>-0.08540533011966255</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.03684531942062255</v>
+        <v>-0.03617703450817352</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.01389885291467547</v>
+        <v>-0.0132267470532359</v>
       </c>
       <c r="E10" t="n">
-        <v>-0.01375131353696614</v>
+        <v>-0.01262775478949569</v>
       </c>
       <c r="F10" t="n">
-        <v>0.01101427517609716</v>
+        <v>0.01155560914974454</v>
       </c>
       <c r="G10" t="n">
-        <v>0.05625645383519688</v>
+        <v>0.0544330335255718</v>
       </c>
       <c r="H10" t="n">
         <v>200</v>
       </c>
       <c r="I10" t="n">
-        <v>1.419618888102778e-52</v>
+        <v>5.47788039336719e-21</v>
+      </c>
+      <c r="J10" t="n">
+        <v>-0.08540533011966255</v>
+      </c>
+      <c r="K10" t="n">
+        <v>-0.005468585937621951</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0.002774862273547618</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0.002057510756835084</v>
+      </c>
+      <c r="N10" t="n">
+        <v>0.0145047231723208</v>
+      </c>
+      <c r="O10" t="n">
+        <v>0.07980528211271566</v>
+      </c>
+      <c r="P10" t="n">
+        <v>6734</v>
       </c>
     </row>
     <row r="11">
@@ -761,28 +985,49 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-0.05352483104718145</v>
+        <v>-0.05565229976921938</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.03885062617734508</v>
+        <v>-0.03934437829685359</v>
       </c>
       <c r="D11" t="n">
-        <v>0.003373943286182917</v>
+        <v>0.00105239405250114</v>
       </c>
       <c r="E11" t="n">
-        <v>-0.0003144052716194623</v>
+        <v>-0.0008439797533041349</v>
       </c>
       <c r="F11" t="n">
-        <v>0.02425649771733857</v>
+        <v>0.02482467568653964</v>
       </c>
       <c r="G11" t="n">
-        <v>0.07674029834749423</v>
+        <v>0.07668552095574374</v>
       </c>
       <c r="H11" t="n">
         <v>200</v>
       </c>
       <c r="I11" t="n">
-        <v>0.001020792084139241</v>
+        <v>0.006518283331999762</v>
+      </c>
+      <c r="J11" t="n">
+        <v>-0.1189838439431949</v>
+      </c>
+      <c r="K11" t="n">
+        <v>-0.02565724972893901</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0.0001125289579782941</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0.0006430143347795879</v>
+      </c>
+      <c r="N11" t="n">
+        <v>0.02545757169568354</v>
+      </c>
+      <c r="O11" t="n">
+        <v>0.1913939030788641</v>
+      </c>
+      <c r="P11" t="n">
+        <v>6903</v>
       </c>
     </row>
     <row r="12">
@@ -795,25 +1040,46 @@
         <v>-1.042039315478823</v>
       </c>
       <c r="C12" t="n">
-        <v>-0.6482649536919325</v>
+        <v>-0.6715282840876718</v>
       </c>
       <c r="D12" t="n">
-        <v>0.02751574504573836</v>
+        <v>-0.02614459485919053</v>
       </c>
       <c r="E12" t="n">
-        <v>0.1446178776713718</v>
+        <v>0.1329502432007628</v>
       </c>
       <c r="F12" t="n">
         <v>0.8583733731705397</v>
       </c>
       <c r="G12" t="n">
-        <v>1.032744898483025</v>
+        <v>1.036336632584194</v>
       </c>
       <c r="H12" t="n">
         <v>200</v>
       </c>
       <c r="I12" t="n">
-        <v>5.295866800295211e-38</v>
+        <v>1.332930942888955e-23</v>
+      </c>
+      <c r="J12" t="n">
+        <v>-1.194871359244933</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0.4283543112910913</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0.8583733731705397</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0.604435563655066</v>
+      </c>
+      <c r="N12" t="n">
+        <v>0.8583733731705397</v>
+      </c>
+      <c r="O12" t="n">
+        <v>1.39954163705767</v>
+      </c>
+      <c r="P12" t="n">
+        <v>6910</v>
       </c>
     </row>
     <row r="13">
@@ -823,7 +1089,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>-0.07294005355340552</v>
+        <v>-0.07059969384217396</v>
       </c>
       <c r="C13" t="n">
         <v>-0.02371713334137563</v>
@@ -832,19 +1098,40 @@
         <v>-0.003161620178162943</v>
       </c>
       <c r="E13" t="n">
-        <v>0.003736591114862303</v>
+        <v>0.004385605534601118</v>
       </c>
       <c r="F13" t="n">
-        <v>0.03999925422943031</v>
+        <v>0.04175612330059014</v>
       </c>
       <c r="G13" t="n">
-        <v>0.07132865133214839</v>
+        <v>0.07331996295719791</v>
       </c>
       <c r="H13" t="n">
         <v>200</v>
       </c>
       <c r="I13" t="n">
-        <v>3.117599858121158e-30</v>
+        <v>0.01901244136103362</v>
+      </c>
+      <c r="J13" t="n">
+        <v>-0.2433615720766874</v>
+      </c>
+      <c r="K13" t="n">
+        <v>-0.02774515941755164</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0.002654529160939341</v>
+      </c>
+      <c r="M13" t="n">
+        <v>-0.00103519648499007</v>
+      </c>
+      <c r="N13" t="n">
+        <v>0.02730036428261405</v>
+      </c>
+      <c r="O13" t="n">
+        <v>0.1364295881383873</v>
+      </c>
+      <c r="P13" t="n">
+        <v>6908</v>
       </c>
     </row>
     <row r="14">
@@ -854,28 +1141,49 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-0.06325915597625067</v>
+        <v>-0.06270379042062882</v>
       </c>
       <c r="C14" t="n">
         <v>-0.03153550507968616</v>
       </c>
       <c r="D14" t="n">
-        <v>-0.008025014177335437</v>
+        <v>-0.007950071134772731</v>
       </c>
       <c r="E14" t="n">
-        <v>-0.004354654469917996</v>
+        <v>-0.003711860297801951</v>
       </c>
       <c r="F14" t="n">
         <v>0.0171931498592831</v>
       </c>
       <c r="G14" t="n">
-        <v>0.06249498753658968</v>
+        <v>0.06245587198139495</v>
       </c>
       <c r="H14" t="n">
         <v>200</v>
       </c>
       <c r="I14" t="n">
-        <v>5.823180393830414e-73</v>
+        <v>0.002108223687764318</v>
+      </c>
+      <c r="J14" t="n">
+        <v>-0.2913523785093455</v>
+      </c>
+      <c r="K14" t="n">
+        <v>-0.0309456572769145</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0.003138125128625682</v>
+      </c>
+      <c r="M14" t="n">
+        <v>-0.00282932171320446</v>
+      </c>
+      <c r="N14" t="n">
+        <v>0.03015854637158898</v>
+      </c>
+      <c r="O14" t="n">
+        <v>0.1774058908319399</v>
+      </c>
+      <c r="P14" t="n">
+        <v>6906</v>
       </c>
     </row>
     <row r="15">
@@ -885,19 +1193,19 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-0.1661258893403259</v>
+        <v>-0.1709644830729272</v>
       </c>
       <c r="C15" t="n">
-        <v>-0.05337892363849682</v>
+        <v>-0.05260274808638295</v>
       </c>
       <c r="D15" t="n">
-        <v>-0.02649847476806589</v>
+        <v>-0.02510490220609712</v>
       </c>
       <c r="E15" t="n">
-        <v>-0.01295111087257593</v>
+        <v>-0.01152435932611688</v>
       </c>
       <c r="F15" t="n">
-        <v>0.0251073645194152</v>
+        <v>0.02918656948098223</v>
       </c>
       <c r="G15" t="n">
         <v>0.1713224022883044</v>
@@ -906,7 +1214,28 @@
         <v>200</v>
       </c>
       <c r="I15" t="n">
-        <v>1.618585718135362e-28</v>
+        <v>1.182752043263361e-12</v>
+      </c>
+      <c r="J15" t="n">
+        <v>-0.284247286480003</v>
+      </c>
+      <c r="K15" t="n">
+        <v>-0.0296905108283936</v>
+      </c>
+      <c r="L15" t="n">
+        <v>0.01026841949686261</v>
+      </c>
+      <c r="M15" t="n">
+        <v>0.016167617508322</v>
+      </c>
+      <c r="N15" t="n">
+        <v>0.0654892985179803</v>
+      </c>
+      <c r="O15" t="n">
+        <v>0.3096954351870551</v>
+      </c>
+      <c r="P15" t="n">
+        <v>6897</v>
       </c>
     </row>
     <row r="16">
@@ -916,28 +1245,49 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>-0.1253891560616145</v>
+        <v>-0.1322559386783419</v>
       </c>
       <c r="C16" t="n">
-        <v>0.0007496112209938762</v>
+        <v>0.003278670847618281</v>
       </c>
       <c r="D16" t="n">
-        <v>0.06677984275508735</v>
+        <v>0.06402060531888823</v>
       </c>
       <c r="E16" t="n">
-        <v>0.05752199347135019</v>
+        <v>0.05644547341793329</v>
       </c>
       <c r="F16" t="n">
         <v>0.1157772953982579</v>
       </c>
       <c r="G16" t="n">
-        <v>0.2520219517915925</v>
+        <v>0.3129644504408422</v>
       </c>
       <c r="H16" t="n">
         <v>200</v>
       </c>
       <c r="I16" t="n">
-        <v>5.107037289944652e-82</v>
+        <v>4.677494472425604e-05</v>
+      </c>
+      <c r="J16" t="n">
+        <v>-0.6537913957644539</v>
+      </c>
+      <c r="K16" t="n">
+        <v>-0.02778368822318529</v>
+      </c>
+      <c r="L16" t="n">
+        <v>0.07299996085653296</v>
+      </c>
+      <c r="M16" t="n">
+        <v>0.08871501764021869</v>
+      </c>
+      <c r="N16" t="n">
+        <v>0.1635765626931332</v>
+      </c>
+      <c r="O16" t="n">
+        <v>0.6079025755559954</v>
+      </c>
+      <c r="P16" t="n">
+        <v>6904</v>
       </c>
     </row>
     <row r="17">
@@ -947,28 +1297,49 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-0.2308935937636936</v>
+        <v>-0.2315554924769821</v>
       </c>
       <c r="C17" t="n">
         <v>-0.06262089830693389</v>
       </c>
       <c r="D17" t="n">
-        <v>-0.02632906312049059</v>
+        <v>-0.0264690855794135</v>
       </c>
       <c r="E17" t="n">
-        <v>-0.01452289687078423</v>
+        <v>-0.01456582234265159</v>
       </c>
       <c r="F17" t="n">
-        <v>0.01994365017956782</v>
+        <v>0.01897331173284523</v>
       </c>
       <c r="G17" t="n">
-        <v>0.249755792024374</v>
+        <v>0.2369229516457163</v>
       </c>
       <c r="H17" t="n">
         <v>200</v>
       </c>
       <c r="I17" t="n">
-        <v>3.998632806013124e-36</v>
+        <v>1.865398648420286e-12</v>
+      </c>
+      <c r="J17" t="n">
+        <v>-0.9620943730503483</v>
+      </c>
+      <c r="K17" t="n">
+        <v>-0.06162018536356149</v>
+      </c>
+      <c r="L17" t="n">
+        <v>0.01697553172792477</v>
+      </c>
+      <c r="M17" t="n">
+        <v>0.02055117473799602</v>
+      </c>
+      <c r="N17" t="n">
+        <v>0.107530934058224</v>
+      </c>
+      <c r="O17" t="n">
+        <v>0.5976792677292522</v>
+      </c>
+      <c r="P17" t="n">
+        <v>6901</v>
       </c>
     </row>
     <row r="18">
@@ -981,25 +1352,46 @@
         <v>-0.08017170523364701</v>
       </c>
       <c r="C18" t="n">
-        <v>0.03716173850635717</v>
+        <v>0.02768418569693564</v>
       </c>
       <c r="D18" t="n">
-        <v>0.08587025015868345</v>
+        <v>0.08587024363174152</v>
       </c>
       <c r="E18" t="n">
-        <v>0.07213889769010863</v>
+        <v>0.07188784865728365</v>
       </c>
       <c r="F18" t="n">
-        <v>0.1108125646367625</v>
+        <v>0.1156087065194975</v>
       </c>
       <c r="G18" t="n">
-        <v>0.177865566103088</v>
+        <v>0.1778655382880352</v>
       </c>
       <c r="H18" t="n">
         <v>200</v>
       </c>
       <c r="I18" t="n">
-        <v>1.913035781795974e-14</v>
+        <v>2.921008264129148e-10</v>
+      </c>
+      <c r="J18" t="n">
+        <v>-0.4219318465892019</v>
+      </c>
+      <c r="K18" t="n">
+        <v>-0.0269627483322332</v>
+      </c>
+      <c r="L18" t="n">
+        <v>0.0492173734662422</v>
+      </c>
+      <c r="M18" t="n">
+        <v>0.04094662235187466</v>
+      </c>
+      <c r="N18" t="n">
+        <v>0.1145919150479999</v>
+      </c>
+      <c r="O18" t="n">
+        <v>0.4614069410695808</v>
+      </c>
+      <c r="P18" t="n">
+        <v>6906</v>
       </c>
     </row>
     <row r="19">
@@ -1015,22 +1407,43 @@
         <v>-0.03010384982054628</v>
       </c>
       <c r="D19" t="n">
-        <v>0.03256964230212465</v>
+        <v>0.02830065962369928</v>
       </c>
       <c r="E19" t="n">
-        <v>0.032315934430698</v>
+        <v>0.03759382517445605</v>
       </c>
       <c r="F19" t="n">
-        <v>0.1042683985480489</v>
+        <v>0.1084327667328305</v>
       </c>
       <c r="G19" t="n">
-        <v>0.3009498408479531</v>
+        <v>0.2687497257446907</v>
       </c>
       <c r="H19" t="n">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="I19" t="n">
-        <v>6.93072120835032e-70</v>
+        <v>6.20398768944093e-14</v>
+      </c>
+      <c r="J19" t="n">
+        <v>-1.259972839150054</v>
+      </c>
+      <c r="K19" t="n">
+        <v>-0.1565924115743439</v>
+      </c>
+      <c r="L19" t="n">
+        <v>0.0003477404080785712</v>
+      </c>
+      <c r="M19" t="n">
+        <v>-0.009900980392606864</v>
+      </c>
+      <c r="N19" t="n">
+        <v>0.1447838002162481</v>
+      </c>
+      <c r="O19" t="n">
+        <v>0.8352640731066129</v>
+      </c>
+      <c r="P19" t="n">
+        <v>6899</v>
       </c>
     </row>
     <row r="20">
@@ -1040,19 +1453,19 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>-0.2248852092405775</v>
+        <v>-0.2213335209100941</v>
       </c>
       <c r="C20" t="n">
-        <v>-0.1139231843284641</v>
+        <v>-0.1113167190258477</v>
       </c>
       <c r="D20" t="n">
         <v>-0.04918256117746451</v>
       </c>
       <c r="E20" t="n">
-        <v>-0.05464450055264896</v>
+        <v>-0.05329789125485283</v>
       </c>
       <c r="F20" t="n">
-        <v>-0.002951229389170122</v>
+        <v>0.001877551653109945</v>
       </c>
       <c r="G20" t="n">
         <v>0.1023098602950465</v>
@@ -1061,7 +1474,28 @@
         <v>200</v>
       </c>
       <c r="I20" t="n">
-        <v>6.622915386817412e-20</v>
+        <v>3.606128533111432e-21</v>
+      </c>
+      <c r="J20" t="n">
+        <v>-0.7677141765117381</v>
+      </c>
+      <c r="K20" t="n">
+        <v>-0.0669818977880924</v>
+      </c>
+      <c r="L20" t="n">
+        <v>0.01658163718647526</v>
+      </c>
+      <c r="M20" t="n">
+        <v>0.02075485381957906</v>
+      </c>
+      <c r="N20" t="n">
+        <v>0.1050809251676018</v>
+      </c>
+      <c r="O20" t="n">
+        <v>0.6230130424571895</v>
+      </c>
+      <c r="P20" t="n">
+        <v>6906</v>
       </c>
     </row>
     <row r="21">
@@ -1080,7 +1514,7 @@
         <v>-0.1082803685755991</v>
       </c>
       <c r="E21" t="n">
-        <v>-0.06739293567155649</v>
+        <v>-0.06612745775368702</v>
       </c>
       <c r="F21" t="n">
         <v>-0.1082803685755991</v>
@@ -1092,7 +1526,28 @@
         <v>200</v>
       </c>
       <c r="I21" t="n">
-        <v>0.008412755718113779</v>
+        <v>0.1778961086889484</v>
+      </c>
+      <c r="J21" t="n">
+        <v>-1.410999778203093</v>
+      </c>
+      <c r="K21" t="n">
+        <v>-0.1082803685755991</v>
+      </c>
+      <c r="L21" t="n">
+        <v>-0.1082803685755991</v>
+      </c>
+      <c r="M21" t="n">
+        <v>-0.03193870619606547</v>
+      </c>
+      <c r="N21" t="n">
+        <v>-0.1082803685755991</v>
+      </c>
+      <c r="O21" t="n">
+        <v>2.560045970396408</v>
+      </c>
+      <c r="P21" t="n">
+        <v>6910</v>
       </c>
     </row>
     <row r="22">
@@ -1105,25 +1560,46 @@
         <v>-0.2992095323766829</v>
       </c>
       <c r="C22" t="n">
-        <v>-0.1541620915477644</v>
+        <v>-0.1636603552523447</v>
       </c>
       <c r="D22" t="n">
-        <v>0.01305119075602768</v>
+        <v>0.002146982303964232</v>
       </c>
       <c r="E22" t="n">
-        <v>-0.001700318786200739</v>
+        <v>-0.006860743827703825</v>
       </c>
       <c r="F22" t="n">
-        <v>0.1179082866268763</v>
+        <v>0.1122762832962423</v>
       </c>
       <c r="G22" t="n">
-        <v>0.3788000894147975</v>
+        <v>0.3842813345778326</v>
       </c>
       <c r="H22" t="n">
         <v>200</v>
       </c>
       <c r="I22" t="n">
-        <v>3.01344311456397e-50</v>
+        <v>7.507610932742241e-07</v>
+      </c>
+      <c r="J22" t="n">
+        <v>-0.9700356528655912</v>
+      </c>
+      <c r="K22" t="n">
+        <v>-0.1657995274777839</v>
+      </c>
+      <c r="L22" t="n">
+        <v>-0.09818738000461348</v>
+      </c>
+      <c r="M22" t="n">
+        <v>0.01187776631456757</v>
+      </c>
+      <c r="N22" t="n">
+        <v>0.1396494305213777</v>
+      </c>
+      <c r="O22" t="n">
+        <v>1.211526828233267</v>
+      </c>
+      <c r="P22" t="n">
+        <v>6906</v>
       </c>
     </row>
     <row r="23">
@@ -1136,25 +1612,46 @@
         <v>-0.07511983617706648</v>
       </c>
       <c r="C23" t="n">
-        <v>-0.02032149580925907</v>
+        <v>-0.01741023089673788</v>
       </c>
       <c r="D23" t="n">
-        <v>0.01634503713643003</v>
+        <v>0.0167511002505765</v>
       </c>
       <c r="E23" t="n">
-        <v>0.01659204201329028</v>
+        <v>0.01595930865457547</v>
       </c>
       <c r="F23" t="n">
-        <v>0.04120440675912406</v>
+        <v>0.03726074347016819</v>
       </c>
       <c r="G23" t="n">
-        <v>0.1533976848071548</v>
+        <v>0.1549806907843769</v>
       </c>
       <c r="H23" t="n">
         <v>200</v>
       </c>
       <c r="I23" t="n">
-        <v>7.5889446895992e-27</v>
+        <v>8.277066225657583e-05</v>
+      </c>
+      <c r="J23" t="n">
+        <v>-0.2185521925595926</v>
+      </c>
+      <c r="K23" t="n">
+        <v>-0.02670961925924831</v>
+      </c>
+      <c r="L23" t="n">
+        <v>0.002634758780145364</v>
+      </c>
+      <c r="M23" t="n">
+        <v>0.002598624538767224</v>
+      </c>
+      <c r="N23" t="n">
+        <v>0.03239959266949494</v>
+      </c>
+      <c r="O23" t="n">
+        <v>0.1660202807468451</v>
+      </c>
+      <c r="P23" t="n">
+        <v>6903</v>
       </c>
     </row>
     <row r="24">
@@ -1164,16 +1661,16 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>-0.9568760905205848</v>
+        <v>-0.87176779529665</v>
       </c>
       <c r="C24" t="n">
-        <v>-0.002191229413592965</v>
+        <v>-0.03577918636303813</v>
       </c>
       <c r="D24" t="n">
-        <v>0.4693344815217594</v>
+        <v>0.3003884891700116</v>
       </c>
       <c r="E24" t="n">
-        <v>0.5163759673252244</v>
+        <v>0.511493708665451</v>
       </c>
       <c r="F24" t="n">
         <v>1.202502669596583</v>
@@ -1185,7 +1682,28 @@
         <v>200</v>
       </c>
       <c r="I24" t="n">
-        <v>4.006623232549932e-29</v>
+        <v>4.025283642438583e-13</v>
+      </c>
+      <c r="J24" t="n">
+        <v>-1.934940026845185</v>
+      </c>
+      <c r="K24" t="n">
+        <v>0.2773206150881414</v>
+      </c>
+      <c r="L24" t="n">
+        <v>1.202502669596583</v>
+      </c>
+      <c r="M24" t="n">
+        <v>0.8251289619143861</v>
+      </c>
+      <c r="N24" t="n">
+        <v>1.202502669596583</v>
+      </c>
+      <c r="O24" t="n">
+        <v>1.840271788547373</v>
+      </c>
+      <c r="P24" t="n">
+        <v>6910</v>
       </c>
     </row>
     <row r="25">
@@ -1204,7 +1722,7 @@
         <v>0.1824614536376945</v>
       </c>
       <c r="E25" t="n">
-        <v>0.1424709370387977</v>
+        <v>0.1409924290992248</v>
       </c>
       <c r="F25" t="n">
         <v>0.1824614536376945</v>
@@ -1216,7 +1734,28 @@
         <v>200</v>
       </c>
       <c r="I25" t="n">
-        <v>0.01853652453348854</v>
+        <v>0.03971825172820997</v>
+      </c>
+      <c r="J25" t="n">
+        <v>-0.9808090168785357</v>
+      </c>
+      <c r="K25" t="n">
+        <v>0.1824614536376945</v>
+      </c>
+      <c r="L25" t="n">
+        <v>0.1824614536376945</v>
+      </c>
+      <c r="M25" t="n">
+        <v>0.1635073902627118</v>
+      </c>
+      <c r="N25" t="n">
+        <v>0.1824614536376945</v>
+      </c>
+      <c r="O25" t="n">
+        <v>1.182846647654198</v>
+      </c>
+      <c r="P25" t="n">
+        <v>6906</v>
       </c>
     </row>
     <row r="26">
@@ -1229,25 +1768,46 @@
         <v>-0.03823447527049852</v>
       </c>
       <c r="C26" t="n">
-        <v>0.01411756498211729</v>
+        <v>0.01231488814045431</v>
       </c>
       <c r="D26" t="n">
-        <v>0.03637041385052315</v>
+        <v>0.03581316777746349</v>
       </c>
       <c r="E26" t="n">
-        <v>0.03882834404137663</v>
+        <v>0.03680331926262733</v>
       </c>
       <c r="F26" t="n">
         <v>0.06056507760307107</v>
       </c>
       <c r="G26" t="n">
-        <v>0.1103008786318144</v>
+        <v>0.102696389649466</v>
       </c>
       <c r="H26" t="n">
         <v>200</v>
       </c>
       <c r="I26" t="n">
-        <v>2.207243903748469e-16</v>
+        <v>4.270750275461512e-09</v>
+      </c>
+      <c r="J26" t="n">
+        <v>-0.4339762674737471</v>
+      </c>
+      <c r="K26" t="n">
+        <v>-0.01284730137197115</v>
+      </c>
+      <c r="L26" t="n">
+        <v>0.02712575111808788</v>
+      </c>
+      <c r="M26" t="n">
+        <v>0.01894631012978134</v>
+      </c>
+      <c r="N26" t="n">
+        <v>0.06487624428987898</v>
+      </c>
+      <c r="O26" t="n">
+        <v>0.3076183804067497</v>
+      </c>
+      <c r="P26" t="n">
+        <v>6906</v>
       </c>
     </row>
     <row r="27">
@@ -1260,25 +1820,46 @@
         <v>-0.09235472125025257</v>
       </c>
       <c r="C27" t="n">
-        <v>-0.02954214440750757</v>
+        <v>-0.03211130317417488</v>
       </c>
       <c r="D27" t="n">
-        <v>-0.01442361107570917</v>
+        <v>-0.01363245319139933</v>
       </c>
       <c r="E27" t="n">
-        <v>-0.01252535803392482</v>
+        <v>-0.01367273635128309</v>
       </c>
       <c r="F27" t="n">
-        <v>0.01533021220233443</v>
+        <v>0.01445536995583023</v>
       </c>
       <c r="G27" t="n">
-        <v>0.06136699720268831</v>
+        <v>0.08560772069108434</v>
       </c>
       <c r="H27" t="n">
         <v>200</v>
       </c>
       <c r="I27" t="n">
-        <v>3.796538929084282e-47</v>
+        <v>1.221932171959567e-19</v>
+      </c>
+      <c r="J27" t="n">
+        <v>-0.4241590167707959</v>
+      </c>
+      <c r="K27" t="n">
+        <v>-0.02163634424329124</v>
+      </c>
+      <c r="L27" t="n">
+        <v>0.0177244475491455</v>
+      </c>
+      <c r="M27" t="n">
+        <v>0.009166396826572703</v>
+      </c>
+      <c r="N27" t="n">
+        <v>0.05309646052043458</v>
+      </c>
+      <c r="O27" t="n">
+        <v>0.2392183188367737</v>
+      </c>
+      <c r="P27" t="n">
+        <v>6905</v>
       </c>
     </row>
     <row r="28">
@@ -1288,28 +1869,49 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>-0.2323048639035409</v>
+        <v>-0.2274873985508793</v>
       </c>
       <c r="C28" t="n">
-        <v>-0.02676467898047757</v>
+        <v>-0.01962939462634037</v>
       </c>
       <c r="D28" t="n">
-        <v>0.07724976437091077</v>
+        <v>0.08088766503996636</v>
       </c>
       <c r="E28" t="n">
-        <v>0.07435996829466403</v>
+        <v>0.0758971764238956</v>
       </c>
       <c r="F28" t="n">
         <v>0.1415513845384354</v>
       </c>
       <c r="G28" t="n">
-        <v>0.5980582519290026</v>
+        <v>0.5686198664404092</v>
       </c>
       <c r="H28" t="n">
         <v>200</v>
       </c>
       <c r="I28" t="n">
-        <v>8.225725897880983e-11</v>
+        <v>1.336308130146845e-07</v>
+      </c>
+      <c r="J28" t="n">
+        <v>-1.567263026768169</v>
+      </c>
+      <c r="K28" t="n">
+        <v>-0.1218410155346685</v>
+      </c>
+      <c r="L28" t="n">
+        <v>0.01634139486076155</v>
+      </c>
+      <c r="M28" t="n">
+        <v>0.005548857444931568</v>
+      </c>
+      <c r="N28" t="n">
+        <v>0.1412579378682135</v>
+      </c>
+      <c r="O28" t="n">
+        <v>0.9548720116201116</v>
+      </c>
+      <c r="P28" t="n">
+        <v>6894</v>
       </c>
     </row>
     <row r="29">
@@ -1319,28 +1921,49 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>-1.609437949687021</v>
+        <v>-1.386294361119906</v>
       </c>
       <c r="C29" t="n">
-        <v>0.04338036920115944</v>
+        <v>0.04336990018477867</v>
       </c>
       <c r="D29" t="n">
-        <v>0.1123130469241564</v>
+        <v>0.1129403652631293</v>
       </c>
       <c r="E29" t="n">
-        <v>0.09610966232323345</v>
+        <v>0.09695842048744927</v>
       </c>
       <c r="F29" t="n">
-        <v>0.2495118108741967</v>
+        <v>0.2466459993934068</v>
       </c>
       <c r="G29" t="n">
-        <v>0.8331040741014193</v>
+        <v>1.094563661856504</v>
       </c>
       <c r="H29" t="n">
         <v>200</v>
       </c>
       <c r="I29" t="n">
-        <v>2.130774863244269e-32</v>
+        <v>5.938007193763216e-22</v>
+      </c>
+      <c r="J29" t="n">
+        <v>-6.236369576534597</v>
+      </c>
+      <c r="K29" t="n">
+        <v>-0.2363887257794555</v>
+      </c>
+      <c r="L29" t="n">
+        <v>0.04518217853883207</v>
+      </c>
+      <c r="M29" t="n">
+        <v>-0.005170657415008868</v>
+      </c>
+      <c r="N29" t="n">
+        <v>0.2682640337929274</v>
+      </c>
+      <c r="O29" t="n">
+        <v>4.510859504811141</v>
+      </c>
+      <c r="P29" t="n">
+        <v>6759</v>
       </c>
     </row>
     <row r="30">
@@ -1353,25 +1976,46 @@
         <v>-0.06560169014464114</v>
       </c>
       <c r="C30" t="n">
-        <v>0.02178280314691549</v>
+        <v>0.01856169755574278</v>
       </c>
       <c r="D30" t="n">
-        <v>0.04527152077350242</v>
+        <v>0.04622152266179411</v>
       </c>
       <c r="E30" t="n">
-        <v>0.03868133541037654</v>
+        <v>0.03675260100555956</v>
       </c>
       <c r="F30" t="n">
-        <v>0.06177430315063696</v>
+        <v>0.06329724248802775</v>
       </c>
       <c r="G30" t="n">
-        <v>0.1128927207622413</v>
+        <v>0.1107294520808135</v>
       </c>
       <c r="H30" t="n">
         <v>200</v>
       </c>
       <c r="I30" t="n">
-        <v>1.104866894260873e-10</v>
+        <v>1.526057288529551e-08</v>
+      </c>
+      <c r="J30" t="n">
+        <v>-0.5917274179263764</v>
+      </c>
+      <c r="K30" t="n">
+        <v>-0.01403094218128883</v>
+      </c>
+      <c r="L30" t="n">
+        <v>0.04351846615628446</v>
+      </c>
+      <c r="M30" t="n">
+        <v>0.03023571749809967</v>
+      </c>
+      <c r="N30" t="n">
+        <v>0.0864016966221117</v>
+      </c>
+      <c r="O30" t="n">
+        <v>0.3683249100969832</v>
+      </c>
+      <c r="P30" t="n">
+        <v>6906</v>
       </c>
     </row>
     <row r="31">
@@ -1384,16 +2028,16 @@
         <v>-0.1051969663144681</v>
       </c>
       <c r="C31" t="n">
-        <v>-0.01969891376433896</v>
+        <v>-0.02117661435724036</v>
       </c>
       <c r="D31" t="n">
-        <v>0.007418960981751238</v>
+        <v>0.004302233715842065</v>
       </c>
       <c r="E31" t="n">
-        <v>0.02044633469847798</v>
+        <v>0.01800298336795778</v>
       </c>
       <c r="F31" t="n">
-        <v>0.06871959407159478</v>
+        <v>0.06797875808624455</v>
       </c>
       <c r="G31" t="n">
         <v>0.1619554286596807</v>
@@ -1402,7 +2046,28 @@
         <v>200</v>
       </c>
       <c r="I31" t="n">
-        <v>0.0008981687156534768</v>
+        <v>0.02586703993956781</v>
+      </c>
+      <c r="J31" t="n">
+        <v>-0.5968156894205409</v>
+      </c>
+      <c r="K31" t="n">
+        <v>-0.03801476119921718</v>
+      </c>
+      <c r="L31" t="n">
+        <v>0.02054891377454158</v>
+      </c>
+      <c r="M31" t="n">
+        <v>0.01760510846861932</v>
+      </c>
+      <c r="N31" t="n">
+        <v>0.08336637380090794</v>
+      </c>
+      <c r="O31" t="n">
+        <v>0.3468651611585689</v>
+      </c>
+      <c r="P31" t="n">
+        <v>6905</v>
       </c>
     </row>
     <row r="32">
@@ -1415,25 +2080,46 @@
         <v>-0.05011718731092912</v>
       </c>
       <c r="C32" t="n">
-        <v>0.01290078061256397</v>
+        <v>0.01200753090679988</v>
       </c>
       <c r="D32" t="n">
-        <v>0.03535170175332476</v>
+        <v>0.0341570265870117</v>
       </c>
       <c r="E32" t="n">
-        <v>0.03143248952189236</v>
+        <v>0.02932469864316681</v>
       </c>
       <c r="F32" t="n">
-        <v>0.05060856668378473</v>
+        <v>0.05142065537648262</v>
       </c>
       <c r="G32" t="n">
-        <v>0.08028366332777048</v>
+        <v>0.08839171330956047</v>
       </c>
       <c r="H32" t="n">
         <v>200</v>
       </c>
       <c r="I32" t="n">
-        <v>1.783416667897899e-08</v>
+        <v>1.782971456948447e-06</v>
+      </c>
+      <c r="J32" t="n">
+        <v>-0.5384480852433047</v>
+      </c>
+      <c r="K32" t="n">
+        <v>-0.01035739484784119</v>
+      </c>
+      <c r="L32" t="n">
+        <v>0.03477896450364055</v>
+      </c>
+      <c r="M32" t="n">
+        <v>0.02137414889165324</v>
+      </c>
+      <c r="N32" t="n">
+        <v>0.06810224686992053</v>
+      </c>
+      <c r="O32" t="n">
+        <v>0.3012923889798985</v>
+      </c>
+      <c r="P32" t="n">
+        <v>6906</v>
       </c>
     </row>
     <row r="33">
@@ -1446,25 +2132,46 @@
         <v>-0.2175167852287912</v>
       </c>
       <c r="C33" t="n">
-        <v>-0.04704115448526489</v>
+        <v>-0.03582183889193486</v>
       </c>
       <c r="D33" t="n">
-        <v>0.07130737500082424</v>
+        <v>0.08182997264254786</v>
       </c>
       <c r="E33" t="n">
-        <v>0.06714041734824656</v>
+        <v>0.06844948077122857</v>
       </c>
       <c r="F33" t="n">
-        <v>0.1762457529416914</v>
+        <v>0.1775939847243919</v>
       </c>
       <c r="G33" t="n">
-        <v>0.4920154497847566</v>
+        <v>0.45793416522021</v>
       </c>
       <c r="H33" t="n">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="I33" t="n">
-        <v>4.551369671419169e-16</v>
+        <v>1.486042070704291e-08</v>
+      </c>
+      <c r="J33" t="n">
+        <v>-1.301103096111104</v>
+      </c>
+      <c r="K33" t="n">
+        <v>-0.1033404376730575</v>
+      </c>
+      <c r="L33" t="n">
+        <v>0.002818852055573273</v>
+      </c>
+      <c r="M33" t="n">
+        <v>0.001439256843840163</v>
+      </c>
+      <c r="N33" t="n">
+        <v>0.1035649935831631</v>
+      </c>
+      <c r="O33" t="n">
+        <v>0.6439752983181363</v>
+      </c>
+      <c r="P33" t="n">
+        <v>6891</v>
       </c>
     </row>
     <row r="34">
@@ -1474,28 +2181,49 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>-0.1954784614381435</v>
+        <v>-0.2003726574267857</v>
       </c>
       <c r="C34" t="n">
-        <v>-0.04754347790122675</v>
+        <v>-0.04387840856356356</v>
       </c>
       <c r="D34" t="n">
-        <v>0.06008584058072301</v>
+        <v>0.07679718132447863</v>
       </c>
       <c r="E34" t="n">
-        <v>0.04985894725612786</v>
+        <v>0.05212661732283934</v>
       </c>
       <c r="F34" t="n">
-        <v>0.129510560033179</v>
+        <v>0.1301047994000087</v>
       </c>
       <c r="G34" t="n">
-        <v>0.3162261382147676</v>
+        <v>0.3022613528755551</v>
       </c>
       <c r="H34" t="n">
         <v>200</v>
       </c>
       <c r="I34" t="n">
-        <v>1.178399185780449e-19</v>
+        <v>6.278671091600975e-12</v>
+      </c>
+      <c r="J34" t="n">
+        <v>-0.8773346924422095</v>
+      </c>
+      <c r="K34" t="n">
+        <v>-0.07483194538305715</v>
+      </c>
+      <c r="L34" t="n">
+        <v>-0.005482890638557998</v>
+      </c>
+      <c r="M34" t="n">
+        <v>-0.0008479261730369825</v>
+      </c>
+      <c r="N34" t="n">
+        <v>0.08083346224549509</v>
+      </c>
+      <c r="O34" t="n">
+        <v>0.387483385668899</v>
+      </c>
+      <c r="P34" t="n">
+        <v>6903</v>
       </c>
     </row>
     <row r="35">
@@ -1508,25 +2236,46 @@
         <v>-0.3660511249047546</v>
       </c>
       <c r="C35" t="n">
-        <v>-0.1273044173439946</v>
+        <v>-0.1341683668860857</v>
       </c>
       <c r="D35" t="n">
-        <v>0.02140759797751163</v>
+        <v>0.02441852108180564</v>
       </c>
       <c r="E35" t="n">
-        <v>0.09513893535639616</v>
+        <v>0.09859641215811932</v>
       </c>
       <c r="F35" t="n">
-        <v>0.2431135100260881</v>
+        <v>0.3021595483668174</v>
       </c>
       <c r="G35" t="n">
-        <v>1.08643329341409</v>
+        <v>0.7928402535268435</v>
       </c>
       <c r="H35" t="n">
         <v>199</v>
       </c>
       <c r="I35" t="n">
-        <v>2.663080508570071e-08</v>
+        <v>0.0001617266490605037</v>
+      </c>
+      <c r="J35" t="n">
+        <v>-1.007007028504877</v>
+      </c>
+      <c r="K35" t="n">
+        <v>-0.2160485754948734</v>
+      </c>
+      <c r="L35" t="n">
+        <v>-0.05103638809042847</v>
+      </c>
+      <c r="M35" t="n">
+        <v>-0.006894975913783071</v>
+      </c>
+      <c r="N35" t="n">
+        <v>0.1412156705542463</v>
+      </c>
+      <c r="O35" t="n">
+        <v>1.906312784784841</v>
+      </c>
+      <c r="P35" t="n">
+        <v>6898</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes to be committed: 	modified:   algotrader-repo/main.py 	modified:   algotrader-repo/models/downprojection/expected_returns_90d.xlsx 	modified:   algotrader-repo/src/data/load_from_yfinance.py 	modified:   algotrader-repo/src/data/make_dataset.py 	modified:   algotrader-repo/src/data/merge_assets.py
</commit_message>
<xml_diff>
--- a/algotrader-repo/models/downprojection/expected_returns_90d.xlsx
+++ b/algotrader-repo/models/downprojection/expected_returns_90d.xlsx
@@ -517,49 +517,49 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.1265050405302508</v>
+        <v>-0.1265049616545293</v>
       </c>
       <c r="C2" t="n">
-        <v>0.02798740803096483</v>
+        <v>0.02853621338375339</v>
       </c>
       <c r="D2" t="n">
-        <v>0.1175778209339658</v>
+        <v>0.1024091301113101</v>
       </c>
       <c r="E2" t="n">
-        <v>0.09510147717839937</v>
+        <v>0.09360077737957928</v>
       </c>
       <c r="F2" t="n">
-        <v>0.1633665301904315</v>
+        <v>0.1628725662800658</v>
       </c>
       <c r="G2" t="n">
-        <v>0.3411567014648403</v>
+        <v>0.3519419509067311</v>
       </c>
       <c r="H2" t="n">
         <v>200</v>
       </c>
       <c r="I2" t="n">
-        <v>0.0004234621523382656</v>
+        <v>0.001281777636193803</v>
       </c>
       <c r="J2" t="n">
-        <v>-0.7128912276988006</v>
+        <v>-0.7128912296116475</v>
       </c>
       <c r="K2" t="n">
-        <v>-0.008995531115022078</v>
+        <v>-0.008942363719679717</v>
       </c>
       <c r="L2" t="n">
-        <v>0.09670145975948755</v>
+        <v>0.09641681559378817</v>
       </c>
       <c r="M2" t="n">
-        <v>0.0877476370511667</v>
+        <v>0.08766650881031511</v>
       </c>
       <c r="N2" t="n">
-        <v>0.1946853083055953</v>
+        <v>0.1946852872502821</v>
       </c>
       <c r="O2" t="n">
-        <v>0.799091992791544</v>
+        <v>0.7990922100683189</v>
       </c>
       <c r="P2" t="n">
-        <v>6906</v>
+        <v>6909</v>
       </c>
     </row>
     <row r="3">
@@ -569,28 +569,28 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-1.004254528637929</v>
+        <v>-1.19950829793096</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.5450151586209133</v>
+        <v>-0.596768448599321</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.04893837032341358</v>
+        <v>-0.06557971301642598</v>
       </c>
       <c r="E3" t="n">
-        <v>0.8120696717870111</v>
+        <v>0.777251203336367</v>
       </c>
       <c r="F3" t="n">
         <v>2.362868664365059</v>
       </c>
       <c r="G3" t="n">
-        <v>2.828942759145652</v>
+        <v>2.765287096223761</v>
       </c>
       <c r="H3" t="n">
         <v>200</v>
       </c>
       <c r="I3" t="n">
-        <v>1.502334513986329e-19</v>
+        <v>2.301377443202516e-21</v>
       </c>
       <c r="J3" t="n">
         <v>-1.970100851827858</v>
@@ -602,7 +602,7 @@
         <v>2.362868664365059</v>
       </c>
       <c r="M3" t="n">
-        <v>1.632517749329234</v>
+        <v>1.631838220881442</v>
       </c>
       <c r="N3" t="n">
         <v>2.362868664365059</v>
@@ -621,49 +621,49 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-0.1606715517021195</v>
+        <v>-0.1701554886275414</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0004905227649435368</v>
+        <v>-0.003409087433133428</v>
       </c>
       <c r="D4" t="n">
-        <v>0.04884297901244362</v>
+        <v>0.04884288860317222</v>
       </c>
       <c r="E4" t="n">
-        <v>0.0469784436399546</v>
+        <v>0.04299114204504838</v>
       </c>
       <c r="F4" t="n">
-        <v>0.1305233328569811</v>
+        <v>0.1265416657056664</v>
       </c>
       <c r="G4" t="n">
-        <v>0.2475528231697341</v>
+        <v>0.2482458605376193</v>
       </c>
       <c r="H4" t="n">
         <v>200</v>
       </c>
       <c r="I4" t="n">
-        <v>1.765419703784751e-21</v>
+        <v>1.556444919653362e-18</v>
       </c>
       <c r="J4" t="n">
         <v>-0.6917923287221859</v>
       </c>
       <c r="K4" t="n">
-        <v>0.0004905227649435368</v>
+        <v>0.0004906264221942103</v>
       </c>
       <c r="L4" t="n">
-        <v>0.0004905227649435368</v>
+        <v>0.0004906264221942103</v>
       </c>
       <c r="M4" t="n">
-        <v>0.0112558562944327</v>
+        <v>0.01147992491516432</v>
       </c>
       <c r="N4" t="n">
-        <v>0.03333001620224238</v>
+        <v>0.03351552490383087</v>
       </c>
       <c r="O4" t="n">
-        <v>0.6536035888920079</v>
+        <v>0.6536035843104006</v>
       </c>
       <c r="P4" t="n">
-        <v>6906</v>
+        <v>6909</v>
       </c>
     </row>
     <row r="5">
@@ -679,13 +679,13 @@
         <v>-0.04226984730491904</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.02817055315158657</v>
+        <v>-0.02721944856551378</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.01953953227856854</v>
+        <v>-0.01878354934220932</v>
       </c>
       <c r="F5" t="n">
-        <v>0.006865740074103668</v>
+        <v>0.006537235055538829</v>
       </c>
       <c r="G5" t="n">
         <v>0.06904032557960171</v>
@@ -694,7 +694,7 @@
         <v>200</v>
       </c>
       <c r="I5" t="n">
-        <v>3.890157063537524e-24</v>
+        <v>4.547865678501218e-20</v>
       </c>
       <c r="J5" t="n">
         <v>-0.480714522359086</v>
@@ -706,16 +706,16 @@
         <v>-0.004286593184065727</v>
       </c>
       <c r="M5" t="n">
-        <v>-0.001769025086395777</v>
+        <v>-0.001735081551960893</v>
       </c>
       <c r="N5" t="n">
-        <v>0.02702615387901008</v>
+        <v>0.0272347284306634</v>
       </c>
       <c r="O5" t="n">
         <v>1.804759915703559</v>
       </c>
       <c r="P5" t="n">
-        <v>6909</v>
+        <v>6908</v>
       </c>
     </row>
     <row r="6">
@@ -728,13 +728,13 @@
         <v>-0.5741156638068546</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.2608960287093573</v>
+        <v>-0.2531813978274012</v>
       </c>
       <c r="D6" t="n">
-        <v>0.7461733332485138</v>
+        <v>0.4426882277559119</v>
       </c>
       <c r="E6" t="n">
-        <v>0.5866907526832866</v>
+        <v>0.5746491821839007</v>
       </c>
       <c r="F6" t="n">
         <v>1.402726308520786</v>
@@ -746,19 +746,19 @@
         <v>200</v>
       </c>
       <c r="I6" t="n">
-        <v>1.381025224912823e-22</v>
+        <v>8.509491082397024e-22</v>
       </c>
       <c r="J6" t="n">
         <v>-0.8465190237872344</v>
       </c>
       <c r="K6" t="n">
-        <v>0.4181442436478377</v>
+        <v>0.4170947895647268</v>
       </c>
       <c r="L6" t="n">
         <v>1.402726308520786</v>
       </c>
       <c r="M6" t="n">
-        <v>1.01457803255993</v>
+        <v>1.014141593287027</v>
       </c>
       <c r="N6" t="n">
         <v>1.402726308520786</v>
@@ -777,28 +777,28 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-0.8494158351574298</v>
+        <v>-0.8828250492348002</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.1399514935542799</v>
+        <v>-0.1443768085708213</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.01164840865164129</v>
+        <v>-0.0294224915684597</v>
       </c>
       <c r="E7" t="n">
-        <v>0.04706193396998795</v>
+        <v>0.03107747866381505</v>
       </c>
       <c r="F7" t="n">
-        <v>0.2732943658675587</v>
+        <v>0.2514871900876546</v>
       </c>
       <c r="G7" t="n">
-        <v>1.133634764220366</v>
+        <v>1.303293713832606</v>
       </c>
       <c r="H7" t="n">
         <v>200</v>
       </c>
       <c r="I7" t="n">
-        <v>4.11580350674338e-31</v>
+        <v>1.182745270911708e-29</v>
       </c>
       <c r="J7" t="n">
         <v>-0.971184982592862</v>
@@ -810,10 +810,10 @@
         <v>-0.3352642187046779</v>
       </c>
       <c r="M7" t="n">
-        <v>-0.1152649432677471</v>
+        <v>-0.1149167894357816</v>
       </c>
       <c r="N7" t="n">
-        <v>0.07039262924546211</v>
+        <v>0.0710175305535993</v>
       </c>
       <c r="O7" t="n">
         <v>1.694114229814654</v>
@@ -829,49 +829,49 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-0.05247635345385821</v>
+        <v>-0.06116053787564785</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.01956554635081176</v>
+        <v>-0.02029982656947119</v>
       </c>
       <c r="D8" t="n">
         <v>-0.001315350380615605</v>
       </c>
       <c r="E8" t="n">
-        <v>0.003357729475243577</v>
+        <v>0.004639091077351176</v>
       </c>
       <c r="F8" t="n">
-        <v>0.01283630487301207</v>
+        <v>0.01788137470693969</v>
       </c>
       <c r="G8" t="n">
-        <v>0.1054033449155986</v>
+        <v>0.1257456832259111</v>
       </c>
       <c r="H8" t="n">
         <v>200</v>
       </c>
       <c r="I8" t="n">
-        <v>0.003478627471606414</v>
+        <v>0.0152072858068446</v>
       </c>
       <c r="J8" t="n">
         <v>-0.2585007380338438</v>
       </c>
       <c r="K8" t="n">
-        <v>-0.02388755105583503</v>
+        <v>-0.02388881566611591</v>
       </c>
       <c r="L8" t="n">
-        <v>-0.0002142456511333328</v>
+        <v>-0.0002218253995437954</v>
       </c>
       <c r="M8" t="n">
-        <v>0.001136466846099111</v>
+        <v>0.00112955960151121</v>
       </c>
       <c r="N8" t="n">
-        <v>0.02693515558715022</v>
+        <v>0.02696654891028974</v>
       </c>
       <c r="O8" t="n">
         <v>0.1450303875968654</v>
       </c>
       <c r="P8" t="n">
-        <v>6910</v>
+        <v>6909</v>
       </c>
     </row>
     <row r="9">
@@ -884,16 +884,16 @@
         <v>-0.5288696539920751</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.0307400945708086</v>
+        <v>-0.007229999194087313</v>
       </c>
       <c r="D9" t="n">
-        <v>0.05215938453877618</v>
+        <v>0.05220215601495467</v>
       </c>
       <c r="E9" t="n">
-        <v>0.03375089676710478</v>
+        <v>0.03405836917884422</v>
       </c>
       <c r="F9" t="n">
-        <v>0.101760537121894</v>
+        <v>0.09562025062391206</v>
       </c>
       <c r="G9" t="n">
         <v>0.2933914744316351</v>
@@ -902,19 +902,19 @@
         <v>200</v>
       </c>
       <c r="I9" t="n">
-        <v>0.00735236862467733</v>
+        <v>0.0004724697281683969</v>
       </c>
       <c r="J9" t="n">
         <v>-1.734894842769978</v>
       </c>
       <c r="K9" t="n">
-        <v>-0.07961270423142532</v>
+        <v>-0.07984922702458114</v>
       </c>
       <c r="L9" t="n">
-        <v>0.03981301103870794</v>
+        <v>0.0396780566885897</v>
       </c>
       <c r="M9" t="n">
-        <v>0.01098484635283651</v>
+        <v>0.0109337394607756</v>
       </c>
       <c r="N9" t="n">
         <v>0.1400376213150778</v>
@@ -923,7 +923,7 @@
         <v>1.405342566876112</v>
       </c>
       <c r="P9" t="n">
-        <v>6906</v>
+        <v>6910</v>
       </c>
     </row>
     <row r="10">
@@ -933,19 +933,19 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-0.08540533011966255</v>
+        <v>-0.07478381437825059</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.03617703450817352</v>
+        <v>-0.03385558064626679</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.0132267470532359</v>
+        <v>-0.01156485803217734</v>
       </c>
       <c r="E10" t="n">
-        <v>-0.01262775478949569</v>
+        <v>-0.01108594680313707</v>
       </c>
       <c r="F10" t="n">
-        <v>0.01155560914974454</v>
+        <v>0.01175224249207635</v>
       </c>
       <c r="G10" t="n">
         <v>0.0544330335255718</v>
@@ -954,28 +954,28 @@
         <v>200</v>
       </c>
       <c r="I10" t="n">
-        <v>5.47788039336719e-21</v>
+        <v>5.491570997464854e-21</v>
       </c>
       <c r="J10" t="n">
         <v>-0.08540533011966255</v>
       </c>
       <c r="K10" t="n">
-        <v>-0.005468585937621951</v>
+        <v>-0.005477087741348451</v>
       </c>
       <c r="L10" t="n">
-        <v>0.002774862273547618</v>
+        <v>0.002779955982857926</v>
       </c>
       <c r="M10" t="n">
-        <v>0.002057510756835084</v>
+        <v>0.002071521103810957</v>
       </c>
       <c r="N10" t="n">
-        <v>0.0145047231723208</v>
+        <v>0.01455527914575426</v>
       </c>
       <c r="O10" t="n">
         <v>0.07980528211271566</v>
       </c>
       <c r="P10" t="n">
-        <v>6734</v>
+        <v>6733</v>
       </c>
     </row>
     <row r="11">
@@ -988,37 +988,37 @@
         <v>-0.05565229976921938</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.03934437829685359</v>
+        <v>-0.03952573856923632</v>
       </c>
       <c r="D11" t="n">
-        <v>0.00105239405250114</v>
+        <v>0.00410061778386123</v>
       </c>
       <c r="E11" t="n">
-        <v>-0.0008439797533041349</v>
+        <v>-0.001453868485693996</v>
       </c>
       <c r="F11" t="n">
-        <v>0.02482467568653964</v>
+        <v>0.02416877589673183</v>
       </c>
       <c r="G11" t="n">
-        <v>0.07668552095574374</v>
+        <v>0.07674029834749423</v>
       </c>
       <c r="H11" t="n">
         <v>200</v>
       </c>
       <c r="I11" t="n">
-        <v>0.006518283331999762</v>
+        <v>0.001435609550449518</v>
       </c>
       <c r="J11" t="n">
         <v>-0.1189838439431949</v>
       </c>
       <c r="K11" t="n">
-        <v>-0.02565724972893901</v>
+        <v>-0.02567593546204155</v>
       </c>
       <c r="L11" t="n">
-        <v>0.0001125289579782941</v>
+        <v>0.0001074527342753649</v>
       </c>
       <c r="M11" t="n">
-        <v>0.0006430143347795879</v>
+        <v>0.0006441089186741676</v>
       </c>
       <c r="N11" t="n">
         <v>0.02545757169568354</v>
@@ -1027,7 +1027,7 @@
         <v>0.1913939030788641</v>
       </c>
       <c r="P11" t="n">
-        <v>6903</v>
+        <v>6904</v>
       </c>
     </row>
     <row r="12">
@@ -1037,16 +1037,16 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-1.042039315478823</v>
+        <v>-1.012025650116356</v>
       </c>
       <c r="C12" t="n">
-        <v>-0.6715282840876718</v>
+        <v>-0.6727537301830955</v>
       </c>
       <c r="D12" t="n">
-        <v>-0.02614459485919053</v>
+        <v>-0.05084481023514804</v>
       </c>
       <c r="E12" t="n">
-        <v>0.1329502432007628</v>
+        <v>0.1155347152717189</v>
       </c>
       <c r="F12" t="n">
         <v>0.8583733731705397</v>
@@ -1058,19 +1058,19 @@
         <v>200</v>
       </c>
       <c r="I12" t="n">
-        <v>1.332930942888955e-23</v>
+        <v>6.625229682921901e-26</v>
       </c>
       <c r="J12" t="n">
         <v>-1.194871359244933</v>
       </c>
       <c r="K12" t="n">
-        <v>0.4283543112910913</v>
+        <v>0.4264355183107558</v>
       </c>
       <c r="L12" t="n">
         <v>0.8583733731705397</v>
       </c>
       <c r="M12" t="n">
-        <v>0.604435563655066</v>
+        <v>0.6042072864817388</v>
       </c>
       <c r="N12" t="n">
         <v>0.8583733731705397</v>
@@ -1089,19 +1089,19 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>-0.07059969384217396</v>
+        <v>-0.07294005355340552</v>
       </c>
       <c r="C13" t="n">
         <v>-0.02371713334137563</v>
       </c>
       <c r="D13" t="n">
-        <v>-0.003161620178162943</v>
+        <v>-0.003898416223683772</v>
       </c>
       <c r="E13" t="n">
-        <v>0.004385605534601118</v>
+        <v>0.004481492598868164</v>
       </c>
       <c r="F13" t="n">
-        <v>0.04175612330059014</v>
+        <v>0.04340502607176652</v>
       </c>
       <c r="G13" t="n">
         <v>0.07331996295719791</v>
@@ -1110,7 +1110,7 @@
         <v>200</v>
       </c>
       <c r="I13" t="n">
-        <v>0.01901244136103362</v>
+        <v>0.001833081545607068</v>
       </c>
       <c r="J13" t="n">
         <v>-0.2433615720766874</v>
@@ -1122,10 +1122,10 @@
         <v>0.002654529160939341</v>
       </c>
       <c r="M13" t="n">
-        <v>-0.00103519648499007</v>
+        <v>-0.001024192731586124</v>
       </c>
       <c r="N13" t="n">
-        <v>0.02730036428261405</v>
+        <v>0.02731712645088797</v>
       </c>
       <c r="O13" t="n">
         <v>0.1364295881383873</v>
@@ -1141,19 +1141,19 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-0.06270379042062882</v>
+        <v>-0.05775469213549117</v>
       </c>
       <c r="C14" t="n">
-        <v>-0.03153550507968616</v>
+        <v>-0.03162320319420703</v>
       </c>
       <c r="D14" t="n">
-        <v>-0.007950071134772731</v>
+        <v>-0.003962132213381716</v>
       </c>
       <c r="E14" t="n">
-        <v>-0.003711860297801951</v>
+        <v>-0.002677493012103305</v>
       </c>
       <c r="F14" t="n">
-        <v>0.0171931498592831</v>
+        <v>0.02015009402648271</v>
       </c>
       <c r="G14" t="n">
         <v>0.06245587198139495</v>
@@ -1162,7 +1162,7 @@
         <v>200</v>
       </c>
       <c r="I14" t="n">
-        <v>0.002108223687764318</v>
+        <v>0.003277629946888321</v>
       </c>
       <c r="J14" t="n">
         <v>-0.2913523785093455</v>
@@ -1174,7 +1174,7 @@
         <v>0.003138125128625682</v>
       </c>
       <c r="M14" t="n">
-        <v>-0.00282932171320446</v>
+        <v>-0.002832519801991041</v>
       </c>
       <c r="N14" t="n">
         <v>0.03015854637158898</v>
@@ -1193,28 +1193,28 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-0.1709644830729272</v>
+        <v>-0.1661258893403259</v>
       </c>
       <c r="C15" t="n">
         <v>-0.05260274808638295</v>
       </c>
       <c r="D15" t="n">
-        <v>-0.02510490220609712</v>
+        <v>-0.01793207871826299</v>
       </c>
       <c r="E15" t="n">
-        <v>-0.01152435932611688</v>
+        <v>-0.008922171080769301</v>
       </c>
       <c r="F15" t="n">
-        <v>0.02918656948098223</v>
+        <v>0.03177162110871939</v>
       </c>
       <c r="G15" t="n">
-        <v>0.1713224022883044</v>
+        <v>0.1880606864948813</v>
       </c>
       <c r="H15" t="n">
         <v>200</v>
       </c>
       <c r="I15" t="n">
-        <v>1.182752043263361e-12</v>
+        <v>1.90022476299875e-10</v>
       </c>
       <c r="J15" t="n">
         <v>-0.284247286480003</v>
@@ -1223,19 +1223,19 @@
         <v>-0.0296905108283936</v>
       </c>
       <c r="L15" t="n">
-        <v>0.01026841949686261</v>
+        <v>0.01035425126250151</v>
       </c>
       <c r="M15" t="n">
-        <v>0.016167617508322</v>
+        <v>0.01627696665475722</v>
       </c>
       <c r="N15" t="n">
-        <v>0.0654892985179803</v>
+        <v>0.06565271832074016</v>
       </c>
       <c r="O15" t="n">
         <v>0.3096954351870551</v>
       </c>
       <c r="P15" t="n">
-        <v>6897</v>
+        <v>6900</v>
       </c>
     </row>
     <row r="16">
@@ -1245,49 +1245,49 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>-0.1322559386783419</v>
+        <v>-0.1747619455214979</v>
       </c>
       <c r="C16" t="n">
-        <v>0.003278670847618281</v>
+        <v>0.0007496112209938762</v>
       </c>
       <c r="D16" t="n">
-        <v>0.06402060531888823</v>
+        <v>0.05972484030274451</v>
       </c>
       <c r="E16" t="n">
-        <v>0.05644547341793329</v>
+        <v>0.05624992312220987</v>
       </c>
       <c r="F16" t="n">
         <v>0.1157772953982579</v>
       </c>
       <c r="G16" t="n">
-        <v>0.3129644504408422</v>
+        <v>0.3668428980663205</v>
       </c>
       <c r="H16" t="n">
         <v>200</v>
       </c>
       <c r="I16" t="n">
-        <v>4.677494472425604e-05</v>
+        <v>1.069406981754463e-05</v>
       </c>
       <c r="J16" t="n">
         <v>-0.6537913957644539</v>
       </c>
       <c r="K16" t="n">
-        <v>-0.02778368822318529</v>
+        <v>-0.02766575544294697</v>
       </c>
       <c r="L16" t="n">
-        <v>0.07299996085653296</v>
+        <v>0.07290074748592168</v>
       </c>
       <c r="M16" t="n">
-        <v>0.08871501764021869</v>
+        <v>0.08844369410965836</v>
       </c>
       <c r="N16" t="n">
-        <v>0.1635765626931332</v>
+        <v>0.1635368133888668</v>
       </c>
       <c r="O16" t="n">
         <v>0.6079025755559954</v>
       </c>
       <c r="P16" t="n">
-        <v>6904</v>
+        <v>6907</v>
       </c>
     </row>
     <row r="17">
@@ -1300,46 +1300,46 @@
         <v>-0.2315554924769821</v>
       </c>
       <c r="C17" t="n">
-        <v>-0.06262089830693389</v>
+        <v>-0.06287710145277631</v>
       </c>
       <c r="D17" t="n">
-        <v>-0.0264690855794135</v>
+        <v>-0.02632906312049059</v>
       </c>
       <c r="E17" t="n">
-        <v>-0.01456582234265159</v>
+        <v>-0.01274409415597829</v>
       </c>
       <c r="F17" t="n">
-        <v>0.01897331173284523</v>
+        <v>0.01902375942989063</v>
       </c>
       <c r="G17" t="n">
-        <v>0.2369229516457163</v>
+        <v>0.2548801598810409</v>
       </c>
       <c r="H17" t="n">
         <v>200</v>
       </c>
       <c r="I17" t="n">
-        <v>1.865398648420286e-12</v>
+        <v>9.259563889443819e-12</v>
       </c>
       <c r="J17" t="n">
         <v>-0.9620943730503483</v>
       </c>
       <c r="K17" t="n">
-        <v>-0.06162018536356149</v>
+        <v>-0.06160902529770464</v>
       </c>
       <c r="L17" t="n">
-        <v>0.01697553172792477</v>
+        <v>0.0171280642468359</v>
       </c>
       <c r="M17" t="n">
-        <v>0.02055117473799602</v>
+        <v>0.02063499896626187</v>
       </c>
       <c r="N17" t="n">
-        <v>0.107530934058224</v>
+        <v>0.1075305085787195</v>
       </c>
       <c r="O17" t="n">
         <v>0.5976792677292522</v>
       </c>
       <c r="P17" t="n">
-        <v>6901</v>
+        <v>6905</v>
       </c>
     </row>
     <row r="18">
@@ -1352,46 +1352,46 @@
         <v>-0.08017170523364701</v>
       </c>
       <c r="C18" t="n">
-        <v>0.02768418569693564</v>
+        <v>0.02469471544058256</v>
       </c>
       <c r="D18" t="n">
-        <v>0.08587024363174152</v>
+        <v>0.0857529781552171</v>
       </c>
       <c r="E18" t="n">
-        <v>0.07188784865728365</v>
+        <v>0.07017845911773038</v>
       </c>
       <c r="F18" t="n">
-        <v>0.1156087065194975</v>
+        <v>0.1154104892617414</v>
       </c>
       <c r="G18" t="n">
-        <v>0.1778655382880352</v>
+        <v>0.1778652246990194</v>
       </c>
       <c r="H18" t="n">
         <v>200</v>
       </c>
       <c r="I18" t="n">
-        <v>2.921008264129148e-10</v>
+        <v>1.264495944357855e-08</v>
       </c>
       <c r="J18" t="n">
-        <v>-0.4219318465892019</v>
+        <v>-0.4219320620170631</v>
       </c>
       <c r="K18" t="n">
-        <v>-0.0269627483322332</v>
+        <v>-0.02679505884958691</v>
       </c>
       <c r="L18" t="n">
-        <v>0.0492173734662422</v>
+        <v>0.04936857686268065</v>
       </c>
       <c r="M18" t="n">
-        <v>0.04094662235187466</v>
+        <v>0.04105440772434405</v>
       </c>
       <c r="N18" t="n">
-        <v>0.1145919150479999</v>
+        <v>0.1146413059504812</v>
       </c>
       <c r="O18" t="n">
-        <v>0.4614069410695808</v>
+        <v>0.4614068755858439</v>
       </c>
       <c r="P18" t="n">
-        <v>6906</v>
+        <v>6909</v>
       </c>
     </row>
     <row r="19">
@@ -1401,49 +1401,49 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>-0.1951696807194789</v>
+        <v>-0.2088877292602151</v>
       </c>
       <c r="C19" t="n">
-        <v>-0.03010384982054628</v>
+        <v>-0.02553030985410783</v>
       </c>
       <c r="D19" t="n">
-        <v>0.02830065962369928</v>
+        <v>0.03666104891639845</v>
       </c>
       <c r="E19" t="n">
-        <v>0.03759382517445605</v>
+        <v>0.04759683329206695</v>
       </c>
       <c r="F19" t="n">
-        <v>0.1084327667328305</v>
+        <v>0.1173897587114444</v>
       </c>
       <c r="G19" t="n">
-        <v>0.2687497257446907</v>
+        <v>0.2962941367093349</v>
       </c>
       <c r="H19" t="n">
         <v>200</v>
       </c>
       <c r="I19" t="n">
-        <v>6.20398768944093e-14</v>
+        <v>4.687786294847794e-16</v>
       </c>
       <c r="J19" t="n">
         <v>-1.259972839150054</v>
       </c>
       <c r="K19" t="n">
-        <v>-0.1565924115743439</v>
+        <v>-0.1568079696316656</v>
       </c>
       <c r="L19" t="n">
-        <v>0.0003477404080785712</v>
+        <v>-0.0006779978254897023</v>
       </c>
       <c r="M19" t="n">
-        <v>-0.009900980392606864</v>
+        <v>-0.01006797161480786</v>
       </c>
       <c r="N19" t="n">
-        <v>0.1447838002162481</v>
+        <v>0.1445331612428419</v>
       </c>
       <c r="O19" t="n">
         <v>0.8352640731066129</v>
       </c>
       <c r="P19" t="n">
-        <v>6899</v>
+        <v>6903</v>
       </c>
     </row>
     <row r="20">
@@ -1453,49 +1453,49 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>-0.2213335209100941</v>
+        <v>-0.203949672127379</v>
       </c>
       <c r="C20" t="n">
-        <v>-0.1113167190258477</v>
+        <v>-0.1011790829168012</v>
       </c>
       <c r="D20" t="n">
-        <v>-0.04918256117746451</v>
+        <v>-0.05734882806348106</v>
       </c>
       <c r="E20" t="n">
-        <v>-0.05329789125485283</v>
+        <v>-0.04952547304990135</v>
       </c>
       <c r="F20" t="n">
-        <v>0.001877551653109945</v>
+        <v>0.003139378866327827</v>
       </c>
       <c r="G20" t="n">
-        <v>0.1023098602950465</v>
+        <v>0.137425626687163</v>
       </c>
       <c r="H20" t="n">
         <v>200</v>
       </c>
       <c r="I20" t="n">
-        <v>3.606128533111432e-21</v>
+        <v>7.301514834631383e-19</v>
       </c>
       <c r="J20" t="n">
         <v>-0.7677141765117381</v>
       </c>
       <c r="K20" t="n">
-        <v>-0.0669818977880924</v>
+        <v>-0.06696387024491396</v>
       </c>
       <c r="L20" t="n">
-        <v>0.01658163718647526</v>
+        <v>0.01664717608915705</v>
       </c>
       <c r="M20" t="n">
-        <v>0.02075485381957906</v>
+        <v>0.02086648676322726</v>
       </c>
       <c r="N20" t="n">
-        <v>0.1050809251676018</v>
+        <v>0.1057295025117775</v>
       </c>
       <c r="O20" t="n">
         <v>0.6230130424571895</v>
       </c>
       <c r="P20" t="n">
-        <v>6906</v>
+        <v>6910</v>
       </c>
     </row>
     <row r="21">
@@ -1514,19 +1514,19 @@
         <v>-0.1082803685755991</v>
       </c>
       <c r="E21" t="n">
-        <v>-0.06612745775368702</v>
+        <v>-0.06679160055894626</v>
       </c>
       <c r="F21" t="n">
         <v>-0.1082803685755991</v>
       </c>
       <c r="G21" t="n">
-        <v>0.2246201345844816</v>
+        <v>0.2230202305397458</v>
       </c>
       <c r="H21" t="n">
         <v>200</v>
       </c>
       <c r="I21" t="n">
-        <v>0.1778961086889484</v>
+        <v>0.1716715065862001</v>
       </c>
       <c r="J21" t="n">
         <v>-1.410999778203093</v>
@@ -1538,7 +1538,7 @@
         <v>-0.1082803685755991</v>
       </c>
       <c r="M21" t="n">
-        <v>-0.03193870619606547</v>
+        <v>-0.03124578666478475</v>
       </c>
       <c r="N21" t="n">
         <v>-0.1082803685755991</v>
@@ -1560,25 +1560,25 @@
         <v>-0.2992095323766829</v>
       </c>
       <c r="C22" t="n">
-        <v>-0.1636603552523447</v>
+        <v>-0.159319791375882</v>
       </c>
       <c r="D22" t="n">
-        <v>0.002146982303964232</v>
+        <v>-0.0129527198737435</v>
       </c>
       <c r="E22" t="n">
-        <v>-0.006860743827703825</v>
+        <v>-0.01140929096836885</v>
       </c>
       <c r="F22" t="n">
-        <v>0.1122762832962423</v>
+        <v>0.1069907807705393</v>
       </c>
       <c r="G22" t="n">
-        <v>0.3842813345778326</v>
+        <v>0.4176061136118215</v>
       </c>
       <c r="H22" t="n">
         <v>200</v>
       </c>
       <c r="I22" t="n">
-        <v>7.507610932742241e-07</v>
+        <v>1.759999624536256e-06</v>
       </c>
       <c r="J22" t="n">
         <v>-0.9700356528655912</v>
@@ -1587,19 +1587,19 @@
         <v>-0.1657995274777839</v>
       </c>
       <c r="L22" t="n">
-        <v>-0.09818738000461348</v>
+        <v>-0.09807771953794429</v>
       </c>
       <c r="M22" t="n">
-        <v>0.01187776631456757</v>
+        <v>0.01189585706781395</v>
       </c>
       <c r="N22" t="n">
-        <v>0.1396494305213777</v>
+        <v>0.1393549936868443</v>
       </c>
       <c r="O22" t="n">
         <v>1.211526828233267</v>
       </c>
       <c r="P22" t="n">
-        <v>6906</v>
+        <v>6909</v>
       </c>
     </row>
     <row r="23">
@@ -1609,19 +1609,19 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>-0.07511983617706648</v>
+        <v>-0.07142057072895883</v>
       </c>
       <c r="C23" t="n">
-        <v>-0.01741023089673788</v>
+        <v>-0.01722118877507506</v>
       </c>
       <c r="D23" t="n">
-        <v>0.0167511002505765</v>
+        <v>0.01715716336472297</v>
       </c>
       <c r="E23" t="n">
-        <v>0.01595930865457547</v>
+        <v>0.01455984543019206</v>
       </c>
       <c r="F23" t="n">
-        <v>0.03726074347016819</v>
+        <v>0.03512285667565352</v>
       </c>
       <c r="G23" t="n">
         <v>0.1549806907843769</v>
@@ -1630,28 +1630,28 @@
         <v>200</v>
       </c>
       <c r="I23" t="n">
-        <v>8.277066225657583e-05</v>
+        <v>0.0002730693857266783</v>
       </c>
       <c r="J23" t="n">
         <v>-0.2185521925595926</v>
       </c>
       <c r="K23" t="n">
-        <v>-0.02670961925924831</v>
+        <v>-0.02682790270134397</v>
       </c>
       <c r="L23" t="n">
         <v>0.002634758780145364</v>
       </c>
       <c r="M23" t="n">
-        <v>0.002598624538767224</v>
+        <v>0.002547134979310592</v>
       </c>
       <c r="N23" t="n">
-        <v>0.03239959266949494</v>
+        <v>0.03238583600737498</v>
       </c>
       <c r="O23" t="n">
         <v>0.1660202807468451</v>
       </c>
       <c r="P23" t="n">
-        <v>6903</v>
+        <v>6907</v>
       </c>
     </row>
     <row r="24">
@@ -1664,37 +1664,37 @@
         <v>-0.87176779529665</v>
       </c>
       <c r="C24" t="n">
-        <v>-0.03577918636303813</v>
+        <v>-0.01743800118957455</v>
       </c>
       <c r="D24" t="n">
-        <v>0.3003884891700116</v>
+        <v>0.1789988202843775</v>
       </c>
       <c r="E24" t="n">
-        <v>0.511493708665451</v>
+        <v>0.5057321490656972</v>
       </c>
       <c r="F24" t="n">
         <v>1.202502669596583</v>
       </c>
       <c r="G24" t="n">
-        <v>1.691182209244244</v>
+        <v>1.639377231146992</v>
       </c>
       <c r="H24" t="n">
         <v>200</v>
       </c>
       <c r="I24" t="n">
-        <v>4.025283642438583e-13</v>
+        <v>4.786156773985488e-14</v>
       </c>
       <c r="J24" t="n">
         <v>-1.934940026845185</v>
       </c>
       <c r="K24" t="n">
-        <v>0.2773206150881414</v>
+        <v>0.2762575963695553</v>
       </c>
       <c r="L24" t="n">
         <v>1.202502669596583</v>
       </c>
       <c r="M24" t="n">
-        <v>0.8251289619143861</v>
+        <v>0.8246615511822273</v>
       </c>
       <c r="N24" t="n">
         <v>1.202502669596583</v>
@@ -1722,7 +1722,7 @@
         <v>0.1824614536376945</v>
       </c>
       <c r="E25" t="n">
-        <v>0.1409924290992248</v>
+        <v>0.1402496076049898</v>
       </c>
       <c r="F25" t="n">
         <v>0.1824614536376945</v>
@@ -1734,7 +1734,7 @@
         <v>200</v>
       </c>
       <c r="I25" t="n">
-        <v>0.03971825172820997</v>
+        <v>0.03722213310130972</v>
       </c>
       <c r="J25" t="n">
         <v>-0.9808090168785357</v>
@@ -1746,7 +1746,7 @@
         <v>0.1824614536376945</v>
       </c>
       <c r="M25" t="n">
-        <v>0.1635073902627118</v>
+        <v>0.1637328115371298</v>
       </c>
       <c r="N25" t="n">
         <v>0.1824614536376945</v>
@@ -1755,7 +1755,7 @@
         <v>1.182846647654198</v>
       </c>
       <c r="P25" t="n">
-        <v>6906</v>
+        <v>6909</v>
       </c>
     </row>
     <row r="26">
@@ -1768,25 +1768,25 @@
         <v>-0.03823447527049852</v>
       </c>
       <c r="C26" t="n">
-        <v>0.01231488814045431</v>
+        <v>0.007659878248659836</v>
       </c>
       <c r="D26" t="n">
-        <v>0.03581316777746349</v>
+        <v>0.03093735772988276</v>
       </c>
       <c r="E26" t="n">
-        <v>0.03680331926262733</v>
+        <v>0.03428601808244843</v>
       </c>
       <c r="F26" t="n">
-        <v>0.06056507760307107</v>
+        <v>0.05935810591168422</v>
       </c>
       <c r="G26" t="n">
-        <v>0.102696389649466</v>
+        <v>0.1018570475598707</v>
       </c>
       <c r="H26" t="n">
         <v>200</v>
       </c>
       <c r="I26" t="n">
-        <v>4.270750275461512e-09</v>
+        <v>6.466923104245808e-07</v>
       </c>
       <c r="J26" t="n">
         <v>-0.4339762674737471</v>
@@ -1795,19 +1795,19 @@
         <v>-0.01284730137197115</v>
       </c>
       <c r="L26" t="n">
-        <v>0.02712575111808788</v>
+        <v>0.02741052071942103</v>
       </c>
       <c r="M26" t="n">
-        <v>0.01894631012978134</v>
+        <v>0.01904359440934204</v>
       </c>
       <c r="N26" t="n">
-        <v>0.06487624428987898</v>
+        <v>0.06512376569208858</v>
       </c>
       <c r="O26" t="n">
         <v>0.3076183804067497</v>
       </c>
       <c r="P26" t="n">
-        <v>6906</v>
+        <v>6909</v>
       </c>
     </row>
     <row r="27">
@@ -1820,46 +1820,46 @@
         <v>-0.09235472125025257</v>
       </c>
       <c r="C27" t="n">
-        <v>-0.03211130317417488</v>
+        <v>-0.0388218946904707</v>
       </c>
       <c r="D27" t="n">
-        <v>-0.01363245319139933</v>
+        <v>-0.01293670495684026</v>
       </c>
       <c r="E27" t="n">
-        <v>-0.01367273635128309</v>
+        <v>-0.01467563863497468</v>
       </c>
       <c r="F27" t="n">
-        <v>0.01445536995583023</v>
+        <v>0.0169079024268269</v>
       </c>
       <c r="G27" t="n">
-        <v>0.08560772069108434</v>
+        <v>0.08422383712096604</v>
       </c>
       <c r="H27" t="n">
         <v>200</v>
       </c>
       <c r="I27" t="n">
-        <v>1.221932171959567e-19</v>
+        <v>8.818356933100744e-19</v>
       </c>
       <c r="J27" t="n">
         <v>-0.4241590167707959</v>
       </c>
       <c r="K27" t="n">
-        <v>-0.02163634424329124</v>
+        <v>-0.02160931880931424</v>
       </c>
       <c r="L27" t="n">
-        <v>0.0177244475491455</v>
+        <v>0.01777330854493266</v>
       </c>
       <c r="M27" t="n">
-        <v>0.009166396826572703</v>
+        <v>0.009172352161423357</v>
       </c>
       <c r="N27" t="n">
-        <v>0.05309646052043458</v>
+        <v>0.05303905048856935</v>
       </c>
       <c r="O27" t="n">
         <v>0.2392183188367737</v>
       </c>
       <c r="P27" t="n">
-        <v>6905</v>
+        <v>6909</v>
       </c>
     </row>
     <row r="28">
@@ -1878,40 +1878,40 @@
         <v>0.08088766503996636</v>
       </c>
       <c r="E28" t="n">
-        <v>0.0758971764238956</v>
+        <v>0.07279143765488696</v>
       </c>
       <c r="F28" t="n">
-        <v>0.1415513845384354</v>
+        <v>0.1356362606492305</v>
       </c>
       <c r="G28" t="n">
-        <v>0.5686198664404092</v>
+        <v>0.5980582519290026</v>
       </c>
       <c r="H28" t="n">
         <v>200</v>
       </c>
       <c r="I28" t="n">
-        <v>1.336308130146845e-07</v>
+        <v>4.593828121474255e-07</v>
       </c>
       <c r="J28" t="n">
         <v>-1.567263026768169</v>
       </c>
       <c r="K28" t="n">
-        <v>-0.1218410155346685</v>
+        <v>-0.122422191722289</v>
       </c>
       <c r="L28" t="n">
-        <v>0.01634139486076155</v>
+        <v>0.0162835467104736</v>
       </c>
       <c r="M28" t="n">
-        <v>0.005548857444931568</v>
+        <v>0.005447518647579029</v>
       </c>
       <c r="N28" t="n">
-        <v>0.1412579378682135</v>
+        <v>0.1412400690736405</v>
       </c>
       <c r="O28" t="n">
         <v>0.9548720116201116</v>
       </c>
       <c r="P28" t="n">
-        <v>6894</v>
+        <v>6897</v>
       </c>
     </row>
     <row r="29">
@@ -1924,25 +1924,25 @@
         <v>-1.386294361119906</v>
       </c>
       <c r="C29" t="n">
-        <v>0.04336990018477867</v>
+        <v>0.04338036920115944</v>
       </c>
       <c r="D29" t="n">
-        <v>0.1129403652631293</v>
+        <v>0.1146672629447543</v>
       </c>
       <c r="E29" t="n">
-        <v>0.09695842048744927</v>
+        <v>0.1293281293816149</v>
       </c>
       <c r="F29" t="n">
-        <v>0.2466459993934068</v>
+        <v>0.2544839981662347</v>
       </c>
       <c r="G29" t="n">
-        <v>1.094563661856504</v>
+        <v>0.8362479812164983</v>
       </c>
       <c r="H29" t="n">
         <v>200</v>
       </c>
       <c r="I29" t="n">
-        <v>5.938007193763216e-22</v>
+        <v>1.613387264037231e-22</v>
       </c>
       <c r="J29" t="n">
         <v>-6.236369576534597</v>
@@ -1951,10 +1951,10 @@
         <v>-0.2363887257794555</v>
       </c>
       <c r="L29" t="n">
-        <v>0.04518217853883207</v>
+        <v>0.04484348321745169</v>
       </c>
       <c r="M29" t="n">
-        <v>-0.005170657415008868</v>
+        <v>-0.005162223124607016</v>
       </c>
       <c r="N29" t="n">
         <v>0.2682640337929274</v>
@@ -1963,7 +1963,7 @@
         <v>4.510859504811141</v>
       </c>
       <c r="P29" t="n">
-        <v>6759</v>
+        <v>6762</v>
       </c>
     </row>
     <row r="30">
@@ -1976,16 +1976,16 @@
         <v>-0.06560169014464114</v>
       </c>
       <c r="C30" t="n">
-        <v>0.01856169755574278</v>
+        <v>0.01278709330076845</v>
       </c>
       <c r="D30" t="n">
         <v>0.04622152266179411</v>
       </c>
       <c r="E30" t="n">
-        <v>0.03675260100555956</v>
+        <v>0.03471274422824927</v>
       </c>
       <c r="F30" t="n">
-        <v>0.06329724248802775</v>
+        <v>0.06475275482922456</v>
       </c>
       <c r="G30" t="n">
         <v>0.1107294520808135</v>
@@ -1994,19 +1994,19 @@
         <v>200</v>
       </c>
       <c r="I30" t="n">
-        <v>1.526057288529551e-08</v>
+        <v>1.161681008187067e-08</v>
       </c>
       <c r="J30" t="n">
         <v>-0.5917274179263764</v>
       </c>
       <c r="K30" t="n">
-        <v>-0.01403094218128883</v>
+        <v>-0.01398366459801871</v>
       </c>
       <c r="L30" t="n">
-        <v>0.04351846615628446</v>
+        <v>0.04356622662150626</v>
       </c>
       <c r="M30" t="n">
-        <v>0.03023571749809967</v>
+        <v>0.0302729012572907</v>
       </c>
       <c r="N30" t="n">
         <v>0.0864016966221117</v>
@@ -2015,7 +2015,7 @@
         <v>0.3683249100969832</v>
       </c>
       <c r="P30" t="n">
-        <v>6906</v>
+        <v>6909</v>
       </c>
     </row>
     <row r="31">
@@ -2025,49 +2025,49 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>-0.1051969663144681</v>
+        <v>-0.1038620811829645</v>
       </c>
       <c r="C31" t="n">
-        <v>-0.02117661435724036</v>
+        <v>-0.02362562913532924</v>
       </c>
       <c r="D31" t="n">
         <v>0.004302233715842065</v>
       </c>
       <c r="E31" t="n">
-        <v>0.01800298336795778</v>
+        <v>0.01560931063754584</v>
       </c>
       <c r="F31" t="n">
-        <v>0.06797875808624455</v>
+        <v>0.06774067023780447</v>
       </c>
       <c r="G31" t="n">
-        <v>0.1619554286596807</v>
+        <v>0.150653925456171</v>
       </c>
       <c r="H31" t="n">
         <v>200</v>
       </c>
       <c r="I31" t="n">
-        <v>0.02586703993956781</v>
+        <v>0.02478524732274142</v>
       </c>
       <c r="J31" t="n">
         <v>-0.5968156894205409</v>
       </c>
       <c r="K31" t="n">
-        <v>-0.03801476119921718</v>
+        <v>-0.03792307064624578</v>
       </c>
       <c r="L31" t="n">
         <v>0.02054891377454158</v>
       </c>
       <c r="M31" t="n">
-        <v>0.01760510846861932</v>
+        <v>0.01764145331867019</v>
       </c>
       <c r="N31" t="n">
-        <v>0.08336637380090794</v>
+        <v>0.08342099309021511</v>
       </c>
       <c r="O31" t="n">
         <v>0.3468651611585689</v>
       </c>
       <c r="P31" t="n">
-        <v>6905</v>
+        <v>6902</v>
       </c>
     </row>
     <row r="32">
@@ -2080,16 +2080,16 @@
         <v>-0.05011718731092912</v>
       </c>
       <c r="C32" t="n">
-        <v>0.01200753090679988</v>
+        <v>0.007049482233273685</v>
       </c>
       <c r="D32" t="n">
-        <v>0.0341570265870117</v>
+        <v>0.0317126126586616</v>
       </c>
       <c r="E32" t="n">
-        <v>0.02932469864316681</v>
+        <v>0.02696957693125283</v>
       </c>
       <c r="F32" t="n">
-        <v>0.05142065537648262</v>
+        <v>0.04858326654491188</v>
       </c>
       <c r="G32" t="n">
         <v>0.08839171330956047</v>
@@ -2098,28 +2098,28 @@
         <v>200</v>
       </c>
       <c r="I32" t="n">
-        <v>1.782971456948447e-06</v>
+        <v>1.035919176548122e-06</v>
       </c>
       <c r="J32" t="n">
         <v>-0.5384480852433047</v>
       </c>
       <c r="K32" t="n">
-        <v>-0.01035739484784119</v>
+        <v>-0.01034661102773585</v>
       </c>
       <c r="L32" t="n">
-        <v>0.03477896450364055</v>
+        <v>0.03483501436289856</v>
       </c>
       <c r="M32" t="n">
-        <v>0.02137414889165324</v>
+        <v>0.02143629204962485</v>
       </c>
       <c r="N32" t="n">
-        <v>0.06810224686992053</v>
+        <v>0.06828919826793883</v>
       </c>
       <c r="O32" t="n">
         <v>0.3012923889798985</v>
       </c>
       <c r="P32" t="n">
-        <v>6906</v>
+        <v>6909</v>
       </c>
     </row>
     <row r="33">
@@ -2129,49 +2129,49 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>-0.2175167852287912</v>
+        <v>-0.2274797780432722</v>
       </c>
       <c r="C33" t="n">
-        <v>-0.03582183889193486</v>
+        <v>-0.03502425072169805</v>
       </c>
       <c r="D33" t="n">
         <v>0.08182997264254786</v>
       </c>
       <c r="E33" t="n">
-        <v>0.06844948077122857</v>
+        <v>0.06672327806440446</v>
       </c>
       <c r="F33" t="n">
         <v>0.1775939847243919</v>
       </c>
       <c r="G33" t="n">
-        <v>0.45793416522021</v>
+        <v>0.4920154497847566</v>
       </c>
       <c r="H33" t="n">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="I33" t="n">
-        <v>1.486042070704291e-08</v>
+        <v>1.951329127379085e-09</v>
       </c>
       <c r="J33" t="n">
         <v>-1.301103096111104</v>
       </c>
       <c r="K33" t="n">
-        <v>-0.1033404376730575</v>
+        <v>-0.1035583053368123</v>
       </c>
       <c r="L33" t="n">
-        <v>0.002818852055573273</v>
+        <v>0.002796419663273176</v>
       </c>
       <c r="M33" t="n">
-        <v>0.001439256843840163</v>
+        <v>0.001312652079557194</v>
       </c>
       <c r="N33" t="n">
-        <v>0.1035649935831631</v>
+        <v>0.1035053560919928</v>
       </c>
       <c r="O33" t="n">
         <v>0.6439752983181363</v>
       </c>
       <c r="P33" t="n">
-        <v>6891</v>
+        <v>6894</v>
       </c>
     </row>
     <row r="34">
@@ -2181,40 +2181,40 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>-0.2003726574267857</v>
+        <v>-0.2191385629542205</v>
       </c>
       <c r="C34" t="n">
-        <v>-0.04387840856356356</v>
+        <v>-0.03942420668521482</v>
       </c>
       <c r="D34" t="n">
-        <v>0.07679718132447863</v>
+        <v>0.08588690475268056</v>
       </c>
       <c r="E34" t="n">
-        <v>0.05212661732283934</v>
+        <v>0.05312151522317347</v>
       </c>
       <c r="F34" t="n">
-        <v>0.1301047994000087</v>
+        <v>0.1363463494843301</v>
       </c>
       <c r="G34" t="n">
-        <v>0.3022613528755551</v>
+        <v>0.3162261382147676</v>
       </c>
       <c r="H34" t="n">
         <v>200</v>
       </c>
       <c r="I34" t="n">
-        <v>6.278671091600975e-12</v>
+        <v>7.389102178076259e-13</v>
       </c>
       <c r="J34" t="n">
         <v>-0.8773346924422095</v>
       </c>
       <c r="K34" t="n">
-        <v>-0.07483194538305715</v>
+        <v>-0.07517585621071178</v>
       </c>
       <c r="L34" t="n">
-        <v>-0.005482890638557998</v>
+        <v>-0.005630592701202055</v>
       </c>
       <c r="M34" t="n">
-        <v>-0.0008479261730369825</v>
+        <v>-0.0009833498417650892</v>
       </c>
       <c r="N34" t="n">
         <v>0.08083346224549509</v>
@@ -2223,7 +2223,7 @@
         <v>0.387483385668899</v>
       </c>
       <c r="P34" t="n">
-        <v>6903</v>
+        <v>6906</v>
       </c>
     </row>
     <row r="35">
@@ -2233,19 +2233,19 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>-0.3660511249047546</v>
+        <v>-0.4461523750158252</v>
       </c>
       <c r="C35" t="n">
         <v>-0.1341683668860857</v>
       </c>
       <c r="D35" t="n">
-        <v>0.02441852108180564</v>
+        <v>0.08669015705316628</v>
       </c>
       <c r="E35" t="n">
-        <v>0.09859641215811932</v>
+        <v>0.1089296542158845</v>
       </c>
       <c r="F35" t="n">
-        <v>0.3021595483668174</v>
+        <v>0.332838818283151</v>
       </c>
       <c r="G35" t="n">
         <v>0.7928402535268435</v>
@@ -2254,28 +2254,28 @@
         <v>199</v>
       </c>
       <c r="I35" t="n">
-        <v>0.0001617266490605037</v>
+        <v>4.89052377292878e-08</v>
       </c>
       <c r="J35" t="n">
         <v>-1.007007028504877</v>
       </c>
       <c r="K35" t="n">
-        <v>-0.2160485754948734</v>
+        <v>-0.216179503137869</v>
       </c>
       <c r="L35" t="n">
-        <v>-0.05103638809042847</v>
+        <v>-0.05123968799350241</v>
       </c>
       <c r="M35" t="n">
-        <v>-0.006894975913783071</v>
+        <v>-0.007080054788925117</v>
       </c>
       <c r="N35" t="n">
-        <v>0.1412156705542463</v>
+        <v>0.1409614883981342</v>
       </c>
       <c r="O35" t="n">
         <v>1.906312784784841</v>
       </c>
       <c r="P35" t="n">
-        <v>6898</v>
+        <v>6902</v>
       </c>
     </row>
   </sheetData>

</xml_diff>